<commit_message>
Agregado de ventana emergente
</commit_message>
<xml_diff>
--- a/recursos/planilla_standard.xlsx
+++ b/recursos/planilla_standard.xlsx
@@ -5555,7 +5555,7 @@
   <dimension ref="A1:AY82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
@@ -5837,7 +5837,9 @@
           <t>Efectivo y Equivalentes al Efectivo</t>
         </is>
       </c>
-      <c r="B6" s="158" t="n"/>
+      <c r="B6" s="158" t="n">
+        <v>32493414952.22</v>
+      </c>
       <c r="C6" s="114" t="n">
         <v>32493414952.22</v>
       </c>
@@ -5910,7 +5912,9 @@
           <t>Otros activos financieros corrientes</t>
         </is>
       </c>
-      <c r="B7" s="158" t="n"/>
+      <c r="B7" s="158" t="n">
+        <v>0</v>
+      </c>
       <c r="C7" s="114" t="n">
         <v>0</v>
       </c>
@@ -5983,7 +5987,9 @@
           <t>Otros Activos No Financieros, Corriente</t>
         </is>
       </c>
-      <c r="B8" s="158" t="n"/>
+      <c r="B8" s="158" t="n">
+        <v>1230818898.66</v>
+      </c>
       <c r="C8" s="114" t="n">
         <v>1230818898.66</v>
       </c>
@@ -6056,7 +6062,9 @@
           <t>Deudores comerciales y otras cuentas por cobrar corrientes</t>
         </is>
       </c>
-      <c r="B9" s="158" t="n"/>
+      <c r="B9" s="158" t="n">
+        <v>15308078505.2884</v>
+      </c>
       <c r="C9" s="114" t="n">
         <v>15308078505.28844</v>
       </c>
@@ -6127,7 +6135,9 @@
           <t>Cuentas por Cobrar a Entidades Relacionadas, Corriente</t>
         </is>
       </c>
-      <c r="B10" s="158" t="n"/>
+      <c r="B10" s="158" t="n">
+        <v>-1.16415321826935e-10</v>
+      </c>
       <c r="C10" s="138" t="n">
         <v>-1.164153218269348e-10</v>
       </c>
@@ -6202,7 +6212,9 @@
           <t>Inventarios</t>
         </is>
       </c>
-      <c r="B11" s="158" t="n"/>
+      <c r="B11" s="158" t="n">
+        <v>1000125165.56</v>
+      </c>
       <c r="C11" s="114" t="n">
         <v>1000125165.56</v>
       </c>
@@ -6275,7 +6287,9 @@
           <t>Activos biológicos corrientes</t>
         </is>
       </c>
-      <c r="B12" s="158" t="n"/>
+      <c r="B12" s="158" t="n">
+        <v>0</v>
+      </c>
       <c r="C12" s="114" t="n">
         <v>0</v>
       </c>
@@ -6348,7 +6362,9 @@
           <t>Activos por impuestos corrientes</t>
         </is>
       </c>
-      <c r="B13" s="158" t="n"/>
+      <c r="B13" s="158" t="n">
+        <v>2375792829.46</v>
+      </c>
       <c r="C13" s="114" t="n">
         <v>2375792829.46</v>
       </c>
@@ -6505,11 +6521,15 @@
           <t xml:space="preserve">Activos no corrientes o grupos de activos para su disposición clasificados como mantenidos para la venta </t>
         </is>
       </c>
-      <c r="B15" s="164" t="n"/>
+      <c r="B15" s="164" t="n">
+        <v>0</v>
+      </c>
       <c r="C15" s="114" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="114" t="n"/>
+      <c r="D15" s="114" t="n">
+        <v>0</v>
+      </c>
       <c r="E15" s="114" t="n">
         <v>0</v>
       </c>
@@ -6580,11 +6600,15 @@
           <t>Activos no corrientes o grupos de activos para su disposición clasificados como mantenidos para distribuir a los propietarios</t>
         </is>
       </c>
-      <c r="B16" s="164" t="n"/>
+      <c r="B16" s="164" t="n">
+        <v>0</v>
+      </c>
       <c r="C16" s="114" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="114" t="n"/>
+      <c r="D16" s="114" t="n">
+        <v>0</v>
+      </c>
       <c r="E16" s="114" t="n">
         <v>0</v>
       </c>
@@ -6911,7 +6935,9 @@
           <t>Otros activos financieros no corrientes</t>
         </is>
       </c>
-      <c r="B20" s="161" t="n"/>
+      <c r="B20" s="161" t="n">
+        <v>10397155079.081</v>
+      </c>
       <c r="C20" s="169" t="n">
         <v>10397155079.08098</v>
       </c>
@@ -7004,7 +7030,9 @@
           <t>Otros activos no financieros no corrientes</t>
         </is>
       </c>
-      <c r="B21" s="161" t="n"/>
+      <c r="B21" s="161" t="n">
+        <v>8084649734</v>
+      </c>
       <c r="C21" s="114" t="n">
         <v>8084649734</v>
       </c>
@@ -7070,7 +7098,9 @@
           <t>Derechos por cobrar no corrientes</t>
         </is>
       </c>
-      <c r="B22" s="161" t="n"/>
+      <c r="B22" s="161" t="n">
+        <v>0</v>
+      </c>
       <c r="C22" s="114" t="n">
         <v>0</v>
       </c>
@@ -7193,7 +7223,9 @@
           <t>Cuentas por Cobrar a Entidades Relacionadas, No Corriente</t>
         </is>
       </c>
-      <c r="B23" s="161" t="n"/>
+      <c r="B23" s="161" t="n">
+        <v>9732389270.53566</v>
+      </c>
       <c r="C23" s="138" t="n">
         <v>9732389270.535658</v>
       </c>
@@ -7316,7 +7348,9 @@
           <t>Inversiones contabilizadas utilizando el método de la participación</t>
         </is>
       </c>
-      <c r="B24" s="161" t="n"/>
+      <c r="B24" s="161" t="n">
+        <v>9745429649.464661</v>
+      </c>
       <c r="C24" s="123" t="n">
         <v>9745429649.464664</v>
       </c>
@@ -7420,7 +7454,9 @@
           <t>Activos intangibles distintos de la plusvalía</t>
         </is>
       </c>
-      <c r="B25" s="161" t="n"/>
+      <c r="B25" s="161" t="n">
+        <v>1080749265</v>
+      </c>
       <c r="C25" s="114" t="n">
         <v>1080749265</v>
       </c>
@@ -7534,7 +7570,9 @@
           <t>Plusvalía</t>
         </is>
       </c>
-      <c r="B26" s="161" t="n"/>
+      <c r="B26" s="161" t="n">
+        <v>403110</v>
+      </c>
       <c r="C26" s="114" t="n">
         <v>403110</v>
       </c>
@@ -7615,7 +7653,9 @@
           <t>Propiedades, Planta y Equipo</t>
         </is>
       </c>
-      <c r="B27" s="161" t="n"/>
+      <c r="B27" s="161" t="n">
+        <v>17068623227.42</v>
+      </c>
       <c r="C27" s="114" t="n">
         <v>17068623227.42</v>
       </c>
@@ -7687,7 +7727,9 @@
           <t>Activos biológicos, no corrientes</t>
         </is>
       </c>
-      <c r="B28" s="161" t="n"/>
+      <c r="B28" s="161" t="n">
+        <v>0</v>
+      </c>
       <c r="C28" s="114" t="n">
         <v>0</v>
       </c>
@@ -7760,7 +7802,9 @@
           <t>Propiedad de inversión</t>
         </is>
       </c>
-      <c r="B29" s="161" t="n"/>
+      <c r="B29" s="161" t="n">
+        <v>2106581917.46</v>
+      </c>
       <c r="C29" s="114" t="n">
         <v>2106581917.46</v>
       </c>
@@ -7833,7 +7877,9 @@
           <t>Activos por impuestos diferidos</t>
         </is>
       </c>
-      <c r="B30" s="161" t="n"/>
+      <c r="B30" s="161" t="n">
+        <v>2214328962</v>
+      </c>
       <c r="C30" s="114" t="n">
         <v>2214328962</v>
       </c>
@@ -8314,7 +8360,9 @@
           <t>Otros pasivos financieros corrientes</t>
         </is>
       </c>
-      <c r="B37" s="166" t="n"/>
+      <c r="B37" s="166" t="n">
+        <v>2037377107.28</v>
+      </c>
       <c r="C37" s="180" t="n">
         <v>2037377107.28</v>
       </c>
@@ -8399,7 +8447,9 @@
           <t>Cuentas por pagar comerciales y otras cuentas por pagar</t>
         </is>
       </c>
-      <c r="B38" s="158" t="n"/>
+      <c r="B38" s="158" t="n">
+        <v>13083193159.78</v>
+      </c>
       <c r="C38" s="114" t="n">
         <v>13083193159.78</v>
       </c>
@@ -8470,7 +8520,9 @@
           <t>Cuentas por Pagar a Entidades Relacionadas, Corriente</t>
         </is>
       </c>
-      <c r="B39" s="158" t="n"/>
+      <c r="B39" s="158" t="n">
+        <v>-1.90921127796173e-08</v>
+      </c>
       <c r="C39" s="138" t="n">
         <v>-1.909211277961731e-08</v>
       </c>
@@ -8542,7 +8594,9 @@
           <t>Otras provisiones a corto plazo</t>
         </is>
       </c>
-      <c r="B40" s="158" t="n"/>
+      <c r="B40" s="158" t="n">
+        <v>463737719</v>
+      </c>
       <c r="C40" s="114" t="n">
         <v>463737719</v>
       </c>
@@ -8615,7 +8669,9 @@
           <t>Pasivos por Impuestos corrientes</t>
         </is>
       </c>
-      <c r="B41" s="158" t="n"/>
+      <c r="B41" s="158" t="n">
+        <v>1237126797</v>
+      </c>
       <c r="C41" s="114" t="n">
         <v>1237126797</v>
       </c>
@@ -8688,7 +8744,9 @@
           <t>Provisiones corrientes por beneficios a los empleados</t>
         </is>
       </c>
-      <c r="B42" s="158" t="n"/>
+      <c r="B42" s="158" t="n">
+        <v>1272171619</v>
+      </c>
       <c r="C42" s="114" t="n">
         <v>1272171619</v>
       </c>
@@ -8761,7 +8819,9 @@
           <t>Otros pasivos no financieros corrientes</t>
         </is>
       </c>
-      <c r="B43" s="158" t="n"/>
+      <c r="B43" s="158" t="n">
+        <v>1646245921.67</v>
+      </c>
       <c r="C43" s="114" t="n">
         <v>1646245921.67</v>
       </c>
@@ -8920,11 +8980,15 @@
           <t>Pasivos incluidos en grupos de activos para su disposición clasificados como mantenidos para la venta</t>
         </is>
       </c>
-      <c r="B45" s="164" t="n"/>
+      <c r="B45" s="164" t="n">
+        <v>0</v>
+      </c>
       <c r="C45" s="114" t="n">
         <v>0</v>
       </c>
-      <c r="D45" s="114" t="n"/>
+      <c r="D45" s="114" t="n">
+        <v>0</v>
+      </c>
       <c r="E45" s="114" t="n">
         <v>0</v>
       </c>
@@ -9177,7 +9241,9 @@
           <t>Otros pasivos financieros, no corrientes</t>
         </is>
       </c>
-      <c r="B48" s="166" t="n"/>
+      <c r="B48" s="166" t="n">
+        <v>2162755124.11418</v>
+      </c>
       <c r="C48" s="180" t="n">
         <v>2162755124.114185</v>
       </c>
@@ -9269,7 +9335,9 @@
           <t>Pasivos no corrientes</t>
         </is>
       </c>
-      <c r="B49" s="158" t="n"/>
+      <c r="B49" s="158" t="n">
+        <v>908295196</v>
+      </c>
       <c r="C49" s="114" t="n">
         <v>908295196</v>
       </c>
@@ -9336,7 +9404,9 @@
           <t>Cuentas por Pagar a Entidades Relacionadas, no corriente</t>
         </is>
       </c>
-      <c r="B50" s="158" t="n"/>
+      <c r="B50" s="158" t="n">
+        <v>4325775236.51468</v>
+      </c>
       <c r="C50" s="138" t="n">
         <v>4325775236.51468</v>
       </c>
@@ -9434,7 +9504,9 @@
           <t>Otras provisiones a largo plazo</t>
         </is>
       </c>
-      <c r="B51" s="158" t="n"/>
+      <c r="B51" s="158" t="n">
+        <v>128379000</v>
+      </c>
       <c r="C51" s="114" t="n">
         <v>128379000</v>
       </c>
@@ -9531,7 +9603,9 @@
           <t>Pasivo por impuestos diferidos</t>
         </is>
       </c>
-      <c r="B52" s="158" t="n"/>
+      <c r="B52" s="158" t="n">
+        <v>2395398086</v>
+      </c>
       <c r="C52" s="114" t="n">
         <v>2395398086</v>
       </c>
@@ -9604,7 +9678,9 @@
           <t>Provisiones no corrientes por beneficios a los empleados</t>
         </is>
       </c>
-      <c r="B53" s="158" t="n"/>
+      <c r="B53" s="158" t="n">
+        <v>0</v>
+      </c>
       <c r="C53" s="114" t="n">
         <v>0</v>
       </c>
@@ -9678,7 +9754,9 @@
           <t>Otros pasivos no financieros no corrientes</t>
         </is>
       </c>
-      <c r="B54" s="158" t="n"/>
+      <c r="B54" s="158" t="n">
+        <v>274927245</v>
+      </c>
       <c r="C54" s="114" t="n">
         <v>274927245</v>
       </c>
@@ -9974,7 +10052,9 @@
           <t>Capital emitido</t>
         </is>
       </c>
-      <c r="B58" s="161" t="n"/>
+      <c r="B58" s="161" t="n">
+        <v>28743629969</v>
+      </c>
       <c r="C58" s="114" t="n">
         <v>28743629969</v>
       </c>
@@ -10041,7 +10121,9 @@
           <t>Ganancias (pérdidas) acumuladas</t>
         </is>
       </c>
-      <c r="B59" s="161" t="n"/>
+      <c r="B59" s="161" t="n">
+        <v>51023010062</v>
+      </c>
       <c r="C59" s="114" t="n">
         <v>51023010062</v>
       </c>
@@ -10107,7 +10189,9 @@
           <t>Primas de emisión</t>
         </is>
       </c>
-      <c r="B60" s="161" t="n"/>
+      <c r="B60" s="161" t="n">
+        <v>0</v>
+      </c>
       <c r="C60" s="114" t="n">
         <v>0</v>
       </c>
@@ -10174,7 +10258,9 @@
           <t>Acciones propias en cartera</t>
         </is>
       </c>
-      <c r="B61" s="161" t="n"/>
+      <c r="B61" s="161" t="n">
+        <v>0</v>
+      </c>
       <c r="C61" s="114" t="n">
         <v>0</v>
       </c>
@@ -10241,7 +10327,9 @@
           <t>Otras participaciones en el patrimonio</t>
         </is>
       </c>
-      <c r="B62" s="161" t="n"/>
+      <c r="B62" s="161" t="n">
+        <v>0</v>
+      </c>
       <c r="C62" s="114" t="n">
         <v>0</v>
       </c>
@@ -10308,7 +10396,9 @@
           <t>Otras reservas</t>
         </is>
       </c>
-      <c r="B63" s="161" t="n"/>
+      <c r="B63" s="161" t="n">
+        <v>2411552424</v>
+      </c>
       <c r="C63" s="114" t="n">
         <v>2411552424</v>
       </c>
@@ -10486,7 +10576,9 @@
           <t>Participaciones no controladoras</t>
         </is>
       </c>
-      <c r="B65" s="161" t="n"/>
+      <c r="B65" s="161" t="n">
+        <v>724965899.810214</v>
+      </c>
       <c r="C65" s="114" t="n">
         <v>724965899.8102137</v>
       </c>

</xml_diff>

<commit_message>
Preparado para nuevo diseño
</commit_message>
<xml_diff>
--- a/recursos/planilla_standard.xlsx
+++ b/recursos/planilla_standard.xlsx
@@ -38,7 +38,6 @@
     <externalReference r:id="rId28"/>
     <externalReference r:id="rId29"/>
     <externalReference r:id="rId30"/>
-    <externalReference r:id="rId31"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Est M$'!$1:$3</definedName>
@@ -2525,173 +2524,10 @@
     <sheetNames>
       <sheetName val="Estado"/>
       <sheetName val="Resultado"/>
-      <sheetName val="Ctas"/>
-      <sheetName val="Hoja1"/>
-      <sheetName val="Datos"/>
-      <sheetName val="Cta Cte EERR"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="5">
-          <cell r="C5">
-            <v>10202391175</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>8863877124</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>404451725</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>6192039</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>107379955</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>-17279115</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>153102815</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>25579789</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>-6201765</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>-165835498</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>1024616468</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="416">
-          <cell r="D416">
-            <v>443150607</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
-    <sheetNames>
-      <sheetName val="Estado"/>
-      <sheetName val="Resultado"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="6">
-          <cell r="Y6">
-            <v>3826419796.22</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="Y7">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="Y8">
-            <v>244845284.66</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="Y9">
-            <v>3069928738.72</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="Y10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="Y11">
-            <v>17627292.56</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="Y12">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="Y13">
-            <v>954474894.46</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="Y15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="Y16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="Y20">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="Y21">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="Y22">
-            <v>0</v>
-          </cell>
-        </row>
         <row r="23">
-          <cell r="Y23">
-            <v>1923515459.0577</v>
-          </cell>
           <cell r="Z23">
             <v>12600</v>
           </cell>
@@ -2710,9 +2546,6 @@
           </cell>
         </row>
         <row r="24">
-          <cell r="Y24">
-            <v>5256221824.26</v>
-          </cell>
           <cell r="Z24">
             <v>5220283407</v>
           </cell>
@@ -2723,147 +2556,9 @@
             <v>35938417.26</v>
           </cell>
         </row>
-        <row r="25">
-          <cell r="Y25">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="Y26">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="Y27">
-            <v>539360404.42</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="Y28">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="Y29">
-            <v>786972684.46</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="Y30">
-            <v>19876930</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="Y37">
-            <v>881974983.28</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="Y38">
-            <v>3727612560.78</v>
-          </cell>
-        </row>
         <row r="39">
-          <cell r="Y39">
-            <v>305542.02</v>
-          </cell>
           <cell r="Z39">
             <v>305542.02</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="Y40">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="Y41">
-            <v>32963207</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="Y42">
-            <v>73618259</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="Y43">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="Y45">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="Y48">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="Y49">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="Y50">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="Y51">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="Y52">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="Y53">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="Y54">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="Y58">
-            <v>9406623059</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="Y59">
-            <v>1508925219</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="Y60">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="Y61">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="Y62">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="Y63">
-            <v>988753254</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="Y65">
-            <v>18467224.74</v>
           </cell>
         </row>
       </sheetData>
@@ -2944,7 +2639,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -2954,223 +2649,7 @@
       <sheetName val="Dato"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>5387933</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>10444966</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>21855290</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>300360854</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>68798365</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>54248821</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>4965044</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>254808755</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>100000</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>1313272</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>91438527</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>-27011</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="5">
           <cell r="C5">
@@ -3235,7 +2714,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -3246,218 +2725,7 @@
       <sheetName val="Hoja1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>1093191</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>191674</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>17123867</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>175296882</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>3960531</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>35884384</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>30646</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>1087339</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>160686140</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>-22364</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="5">
           <cell r="C5">
@@ -3523,7 +2791,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -3543,16 +2811,6 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4">
-        <row r="15">
-          <cell r="AC15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="AC16">
-            <v>0</v>
-          </cell>
-        </row>
         <row r="65">
           <cell r="AD65">
             <v>-240659.273400002</v>
@@ -3579,7 +2837,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -3594,218 +2852,11 @@
       <sheetName val="NoCon"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="10">
-          <cell r="C10">
-            <v>-1.16415321826935e-10</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="6">
-          <cell r="AC6">
-            <v>19529113800</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="AC7">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="AC8">
-            <v>918103580</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="AC9">
-            <v>8020150772</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="AC11">
-            <v>922381337</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="AC12">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="AC13">
-            <v>632874679</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="AC20">
-            <v>11222624019</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="AC21">
-            <v>16641984</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="AC22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="AC23">
-            <v>6997365974</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="AC24">
-            <v>5275727314</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="AC25">
-            <v>6059</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="AC26">
-            <v>403110</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="AC27">
-            <v>9234185858</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="AC28">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="AC29">
-            <v>98063358</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="AC30">
-            <v>1973899479</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="AC37">
-            <v>558046576</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="AC38">
-            <v>5414028694</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="AC39">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="AC40">
-            <v>463737719</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="AC41">
-            <v>1112722638</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="AC42">
-            <v>932917018</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="AC43">
-            <v>625311782</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="AC45">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="AC48">
-            <v>4652450566</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="AC49">
-            <v>227887275</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="AC50">
-            <v>6806005656</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="AC51">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="AC52">
-            <v>1446182627</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="AC53">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="AC54">
-            <v>93967634</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="AC58">
-            <v>32296318921</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="AC59">
-            <v>7719195458</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="AC60">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="AC61">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="AC62">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="AC63">
-            <v>2488253058</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="AC65">
-            <v>4515701</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5">
         <row r="5">
           <cell r="AC5">
@@ -3898,7 +2949,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -4054,7 +3105,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -4195,7 +3246,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -4420,7 +3471,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -4444,6 +3495,50 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook r:id="rId1">
+    <sheetNames>
+      <sheetName val="6220001 Utilidades empresas rel"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="12">
+          <cell r="N12">
+            <v>10569132</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="N13">
+            <v>23950208</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>890084326</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>952630657</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="N16">
+            <v>338180773</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="N17">
+            <v>631879</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4504,50 +3599,6 @@
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
-      <sheetName val="6220001 Utilidades empresas rel"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="12">
-          <cell r="N12">
-            <v>10569132</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="N13">
-            <v>23950208</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>890084326</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="N15">
-            <v>952630657</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="N16">
-            <v>338180773</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="N17">
-            <v>631879</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
-    <sheetNames>
       <sheetName val="5220001 Perdidas empresas relac"/>
     </sheetNames>
     <sheetDataSet>
@@ -4578,7 +3629,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -4650,35 +3701,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
-    <sheetNames>
-      <sheetName val="Estado"/>
-      <sheetName val="Resultado"/>
-      <sheetName val="Ctas"/>
-      <sheetName val="Dato"/>
-      <sheetName val="Hoja2"/>
-      <sheetName val="Hoja1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="7">
-          <cell r="C7">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -4878,7 +3900,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -4995,7 +4017,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -5016,7 +4038,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -5212,7 +4234,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -5287,7 +4309,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook r:id="rId1">
     <sheetNames>
@@ -5356,6 +4378,101 @@
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook r:id="rId1">
+    <sheetNames>
+      <sheetName val="Estado"/>
+      <sheetName val="Resultado"/>
+      <sheetName val="Ctas"/>
+      <sheetName val="Hoja1"/>
+      <sheetName val="Datos"/>
+      <sheetName val="Cta Cte EERR"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="5">
+          <cell r="C5">
+            <v>10202391175</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>8863877124</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>404451725</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>6192039</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="C15">
+            <v>107379955</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17">
+            <v>-17279115</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="C19">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23">
+            <v>153102815</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>25579789</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>-6201765</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>-165835498</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>1024616468</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="416">
+          <cell r="D416">
+            <v>443150607</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7144,11 +6261,11 @@
   <dimension ref="A1:AY91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D57" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65:F65"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65:J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.4571428571429" defaultRowHeight="12"/>
@@ -7615,13 +6732,11 @@
       <c r="H6" s="129" t="n">
         <v>5387933</v>
       </c>
-      <c r="I6" s="129">
-        <f>+[13]Estado!C6</f>
-        <v/>
-      </c>
-      <c r="J6" s="129">
-        <f>+'[15]Estado$'!$AC$6</f>
-        <v/>
+      <c r="I6" s="129" t="n">
+        <v>1093191</v>
+      </c>
+      <c r="J6" s="129" t="n">
+        <v>19529113800</v>
       </c>
       <c r="K6" s="88" t="n"/>
       <c r="L6" s="129" t="n">
@@ -7680,13 +6795,11 @@
       <c r="H7" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="129">
-        <f>+[3]Estado!C7</f>
-        <v/>
-      </c>
-      <c r="J7" s="129">
-        <f>+'[15]Estado$'!$AC$7</f>
-        <v/>
+      <c r="I7" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K7" s="88" t="n"/>
       <c r="L7" s="129" t="n">
@@ -7745,13 +6858,11 @@
       <c r="H8" s="129" t="n">
         <v>10444966</v>
       </c>
-      <c r="I8" s="129">
-        <f>+[13]Estado!C8</f>
-        <v/>
-      </c>
-      <c r="J8" s="129">
-        <f>+'[15]Estado$'!$AC$8</f>
-        <v/>
+      <c r="I8" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="129" t="n">
+        <v>918103580</v>
       </c>
       <c r="K8" s="88" t="n"/>
       <c r="L8" s="129" t="n">
@@ -7816,17 +6927,15 @@
       <c r="H9" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="129">
-        <f>+[13]Estado!C9</f>
-        <v/>
-      </c>
-      <c r="J9" s="129">
-        <f>+'[15]Estado$'!$AC$9</f>
-        <v/>
+      <c r="I9" s="129" t="n">
+        <v>191674</v>
+      </c>
+      <c r="J9" s="129" t="n">
+        <v>8020150772</v>
       </c>
       <c r="K9" s="88" t="n"/>
       <c r="L9" s="142">
-        <f>+'[18]Detalle Cta Cte  Reclasi(Final)'!$BM$43</f>
+        <f>+'[17]Detalle Cta Cte  Reclasi(Final)'!$BM$43</f>
         <v/>
       </c>
       <c r="M9" s="129" t="n">
@@ -7882,13 +6991,11 @@
       <c r="H10" s="132" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="132">
-        <f>+[13]Estado!C10</f>
-        <v/>
-      </c>
-      <c r="J10" s="132">
-        <f>+'[15]Est US$'!$C$10</f>
-        <v/>
+      <c r="I10" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="132" t="n">
+        <v>0</v>
       </c>
       <c r="K10" s="165" t="n"/>
       <c r="L10" s="132" t="n">
@@ -7947,13 +7054,11 @@
       <c r="H11" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="129">
-        <f>+[13]Estado!C11</f>
-        <v/>
-      </c>
-      <c r="J11" s="129">
-        <f>+'[15]Estado$'!$AC$11</f>
-        <v/>
+      <c r="I11" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="129" t="n">
+        <v>922381337</v>
       </c>
       <c r="K11" s="88" t="n"/>
       <c r="L11" s="129" t="n">
@@ -8012,13 +7117,11 @@
       <c r="H12" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="129">
-        <f>+[13]Estado!C12</f>
-        <v/>
-      </c>
-      <c r="J12" s="129">
-        <f>+'[15]Estado$'!$AC$12</f>
-        <v/>
+      <c r="I12" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K12" s="88" t="n"/>
       <c r="L12" s="129" t="n">
@@ -8077,13 +7180,11 @@
       <c r="H13" s="129" t="n">
         <v>21855290</v>
       </c>
-      <c r="I13" s="129">
-        <f>+[13]Estado!C13</f>
-        <v/>
-      </c>
-      <c r="J13" s="129">
-        <f>+'[15]Estado$'!$AC$13</f>
-        <v/>
+      <c r="I13" s="129" t="n">
+        <v>17123867</v>
+      </c>
+      <c r="J13" s="129" t="n">
+        <v>632874679</v>
       </c>
       <c r="K13" s="88" t="n"/>
       <c r="L13" s="129" t="n">
@@ -8221,13 +7322,11 @@
       <c r="H15" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="129">
-        <f>+[13]Estado!C15</f>
-        <v/>
-      </c>
-      <c r="J15" s="129">
-        <f>+'[14]Estado$'!$AC$15</f>
-        <v/>
+      <c r="I15" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K15" s="88" t="n"/>
       <c r="L15" s="129" t="n">
@@ -8286,13 +7385,11 @@
       <c r="H16" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="129">
-        <f>+[13]Estado!C16</f>
-        <v/>
-      </c>
-      <c r="J16" s="129">
-        <f>+'[14]Estado$'!$AC$16</f>
-        <v/>
+      <c r="I16" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K16" s="88" t="n"/>
       <c r="L16" s="129" t="n">
@@ -8596,13 +7693,11 @@
       <c r="H20" s="139" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="139">
-        <f>+[13]Estado!C20</f>
-        <v/>
-      </c>
-      <c r="J20" s="139">
-        <f>+'[15]Estado$'!$AC$20</f>
-        <v/>
+      <c r="I20" s="139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="139" t="n">
+        <v>11222624019</v>
       </c>
       <c r="K20" s="88" t="n"/>
       <c r="L20" s="139" t="n"/>
@@ -8610,7 +7705,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="139">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$J$55-'[18]cta cte  (Ajustes) (Final)'!$R$55</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$J$55-'[17]cta cte  (Ajustes) (Final)'!$R$55</f>
         <v/>
       </c>
       <c r="O20" s="139" t="n">
@@ -8626,7 +7721,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="139">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AO$55-'[18]cta cte  (Ajustes) (Final)'!$AQ$55</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AO$55-'[17]cta cte  (Ajustes) (Final)'!$AQ$55</f>
         <v/>
       </c>
       <c r="T20" s="129" t="n">
@@ -8638,31 +7733,31 @@
         <v/>
       </c>
       <c r="W20" s="179">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$J$54</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$J$54</f>
         <v/>
       </c>
       <c r="X20" s="180">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$N$49</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$N$49</f>
         <v/>
       </c>
       <c r="Y20" s="204">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$AM$46</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$AM$46</f>
         <v/>
       </c>
       <c r="Z20" s="205">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$AO$47</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$AO$47</f>
         <v/>
       </c>
       <c r="AA20" s="324">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$BI$49</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$BI$49</f>
         <v/>
       </c>
       <c r="AB20" s="325">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$AQ$49</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$AQ$49</f>
         <v/>
       </c>
       <c r="AC20" s="208">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$R$49</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$R$49</f>
         <v/>
       </c>
       <c r="AD20" s="119" t="n"/>
@@ -8707,13 +7802,11 @@
       <c r="H21" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="129">
-        <f>+[13]Estado!C21</f>
-        <v/>
-      </c>
-      <c r="J21" s="129">
-        <f>+'[15]Estado$'!$AC$21</f>
-        <v/>
+      <c r="I21" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="129" t="n">
+        <v>16641984</v>
       </c>
       <c r="K21" s="88" t="n"/>
       <c r="L21" s="167">
@@ -8812,13 +7905,11 @@
       <c r="H22" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="129">
-        <f>+[13]Estado!C22</f>
-        <v/>
-      </c>
-      <c r="J22" s="129">
-        <f>+'[15]Estado$'!$AC$22</f>
-        <v/>
+      <c r="I22" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K22" s="88" t="n"/>
       <c r="M22" s="129" t="n">
@@ -8854,7 +7945,7 @@
         </is>
       </c>
       <c r="X22" s="183">
-        <f>+[16]Estado!$Z$22</f>
+        <f>+[15]Estado!$Z$22</f>
         <v/>
       </c>
       <c r="Y22" s="209" t="inlineStr">
@@ -8910,7 +8001,7 @@
       <c r="AJ22" s="226" t="n"/>
       <c r="AK22" s="227" t="n"/>
       <c r="AL22" s="198">
-        <f>+[6]Estado!$AG$22</f>
+        <f>+[5]Estado!$AG$22</f>
         <v/>
       </c>
       <c r="AM22" s="228" t="inlineStr">
@@ -8929,15 +8020,15 @@
         </is>
       </c>
       <c r="AP22" s="233">
-        <f>+'[5]Estado$'!$AG$22</f>
+        <f>+'[4]Estado$'!$AG$22</f>
         <v/>
       </c>
       <c r="AQ22" s="233">
-        <f>+'[5]Estado$'!$AL$22</f>
+        <f>+'[4]Estado$'!$AL$22</f>
         <v/>
       </c>
       <c r="AR22" s="234">
-        <f>+'[5]Estado$'!$AM$22</f>
+        <f>+'[4]Estado$'!$AM$22</f>
         <v/>
       </c>
       <c r="AS22" s="235" t="inlineStr">
@@ -8946,7 +8037,7 @@
         </is>
       </c>
       <c r="AT22" s="236">
-        <f>+'[5]Estado$'!$AE$22</f>
+        <f>+'[4]Estado$'!$AE$22</f>
         <v/>
       </c>
       <c r="AV22" s="237" t="inlineStr">
@@ -8980,45 +8071,43 @@
       <c r="H23" s="142" t="n">
         <v>300360854</v>
       </c>
-      <c r="I23" s="142">
-        <f>+[13]Estado!C23</f>
-        <v/>
-      </c>
-      <c r="J23" s="142">
-        <f>+'[15]Estado$'!$AC$23</f>
-        <v/>
+      <c r="I23" s="142" t="n">
+        <v>175296882</v>
+      </c>
+      <c r="J23" s="142" t="n">
+        <v>6997365974</v>
       </c>
       <c r="K23" s="168" t="n"/>
       <c r="L23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$B$43-'[18]Detalle Cta Cte  Reclasi(Final)'!$BM$57+417</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$B$43-'[17]Detalle Cta Cte  Reclasi(Final)'!$BM$57+417</f>
         <v/>
       </c>
       <c r="M23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$D$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$D$43</f>
         <v/>
       </c>
       <c r="N23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$F$43-'[18]cta cte  (Ajustes) (Final)'!$H$43-'[18]cta cte  (Ajustes) (Final)'!$T$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$F$43-'[17]cta cte  (Ajustes) (Final)'!$H$43-'[17]cta cte  (Ajustes) (Final)'!$T$43</f>
         <v/>
       </c>
       <c r="O23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AA$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AA$43</f>
         <v/>
       </c>
       <c r="P23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AC$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AC$43</f>
         <v/>
       </c>
       <c r="Q23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AI$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AI$43</f>
         <v/>
       </c>
       <c r="R23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AK$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AK$43</f>
         <v/>
       </c>
       <c r="S23" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AM$43-'[18]cta cte  (Ajustes) (Final)'!$BG$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AM$43-'[17]cta cte  (Ajustes) (Final)'!$BG$43</f>
         <v/>
       </c>
       <c r="T23" s="142" t="n">
@@ -9030,82 +8119,82 @@
         <v/>
       </c>
       <c r="W23" s="175">
-        <f>+[16]Estado!$AE$23</f>
+        <f>+[15]Estado!$AE$23</f>
         <v/>
       </c>
       <c r="X23" s="326">
-        <f>+[16]Estado!$Z$23</f>
+        <f>+[15]Estado!$Z$23</f>
         <v/>
       </c>
       <c r="Y23" s="327">
-        <f>+[7]Ctas!$D$197</f>
+        <f>+[6]Ctas!$D$197</f>
         <v/>
       </c>
       <c r="Z23" s="327">
-        <f>+[7]Ctas!$D$198</f>
+        <f>+[6]Ctas!$D$198</f>
         <v/>
       </c>
       <c r="AA23" s="327">
-        <f>+[7]Ctas!$D$199</f>
+        <f>+[6]Ctas!$D$199</f>
         <v/>
       </c>
       <c r="AB23" s="214" t="n">
         <v>0</v>
       </c>
       <c r="AC23" s="214">
-        <f>+[7]Ctas!$D$208</f>
+        <f>+[6]Ctas!$D$208</f>
         <v/>
       </c>
       <c r="AD23" s="214">
-        <f>+[7]Ctas!$D$211</f>
+        <f>+[6]Ctas!$D$211</f>
         <v/>
       </c>
       <c r="AE23" s="214">
-        <f>+[7]Ctas!$D$220</f>
+        <f>+[6]Ctas!$D$220</f>
         <v/>
       </c>
       <c r="AF23" s="214">
-        <f>+[7]Ctas!$D$235</f>
+        <f>+[6]Ctas!$D$235</f>
         <v/>
       </c>
       <c r="AG23" s="327">
-        <f>+[7]Ctas!$D$228</f>
+        <f>+[6]Ctas!$D$228</f>
         <v/>
       </c>
       <c r="AH23" s="327">
-        <f>+[7]Ctas!$D$230</f>
+        <f>+[6]Ctas!$D$230</f>
         <v/>
       </c>
       <c r="AJ23" s="226" t="n"/>
       <c r="AK23" s="226" t="n"/>
       <c r="AL23" s="199">
-        <f>+[11]Estado!$AH$23</f>
+        <f>+[10]Estado!$AH$23</f>
         <v/>
       </c>
       <c r="AM23" s="328">
-        <f>+[11]Estado!$Z$23</f>
+        <f>+[10]Estado!$Z$23</f>
         <v/>
       </c>
       <c r="AN23" s="328">
-        <f>+[11]Estado!$AB$23</f>
+        <f>+[10]Estado!$AB$23</f>
         <v/>
       </c>
       <c r="AO23" s="326">
-        <f>+[11]Estado!$AC$23</f>
+        <f>+[10]Estado!$AC$23</f>
         <v/>
       </c>
       <c r="AP23" s="234" t="n"/>
       <c r="AQ23" s="234">
-        <f>+'[17]Estado$'!$AL$23+'[17]Estado$'!$AP$23+'[17]Estado$'!$AR$23</f>
+        <f>+'[16]Estado$'!$AL$23+'[16]Estado$'!$AP$23+'[16]Estado$'!$AR$23</f>
         <v/>
       </c>
       <c r="AR23" s="234" t="n"/>
       <c r="AS23" s="329">
-        <f>+'[17]Estado$'!$AN$23</f>
+        <f>+'[16]Estado$'!$AN$23</f>
         <v/>
       </c>
       <c r="AT23" s="234">
-        <f>+'[17]Estado$'!$AE$23</f>
+        <f>+'[16]Estado$'!$AE$23</f>
         <v/>
       </c>
       <c r="AU23" s="326" t="n"/>
@@ -9118,7 +8207,7 @@
         <v/>
       </c>
       <c r="AX23" s="119">
-        <f>+'[18]Detalle Cta Cte  Reclasi(Final)'!$BM$43</f>
+        <f>+'[17]Detalle Cta Cte  Reclasi(Final)'!$BM$43</f>
         <v/>
       </c>
       <c r="AY23" s="119">
@@ -9151,29 +8240,27 @@
       <c r="H24" s="144" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="144">
-        <f>+[13]Estado!C24</f>
-        <v/>
-      </c>
-      <c r="J24" s="144">
-        <f>+'[15]Estado$'!$AC$24</f>
-        <v/>
+      <c r="I24" s="144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="144" t="n">
+        <v>5275727314</v>
       </c>
       <c r="K24" s="88" t="n"/>
       <c r="L24" s="169">
-        <f>-'[19]Invers. Ajuste Consol.'!$B$40</f>
+        <f>-'[18]Invers. Ajuste Consol.'!$B$40</f>
         <v/>
       </c>
       <c r="M24" s="167" t="n"/>
       <c r="N24" s="169">
-        <f>-[16]Estado!$Y$24</f>
+        <f>-[15]Estado!$Y$24</f>
         <v/>
       </c>
       <c r="O24" s="169" t="n">
         <v>0</v>
       </c>
       <c r="P24" s="169">
-        <f>-[11]Estado!$Z$24-[11]Estado!$AB$24</f>
+        <f>-[10]Estado!$Z$24-[10]Estado!$AB$24</f>
         <v/>
       </c>
       <c r="Q24" s="169" t="n">
@@ -9183,7 +8270,7 @@
         <v>0</v>
       </c>
       <c r="S24" s="169">
-        <f>-'[17]Estado$'!$AL$24</f>
+        <f>-'[16]Estado$'!$AL$24</f>
         <v/>
       </c>
       <c r="T24" s="169">
@@ -9196,43 +8283,43 @@
         <v/>
       </c>
       <c r="W24" s="175">
-        <f>+[7]Ctas!$D$257</f>
+        <f>+[6]Ctas!$D$257</f>
         <v/>
       </c>
       <c r="X24" s="175">
-        <f>+[7]Ctas!$D$256</f>
+        <f>+[6]Ctas!$D$256</f>
         <v/>
       </c>
       <c r="Y24" s="119">
-        <f>+[7]Ctas!$D$249</f>
+        <f>+[6]Ctas!$D$249</f>
         <v/>
       </c>
       <c r="Z24" s="119">
-        <f>+[7]Ctas!$D$243</f>
+        <f>+[6]Ctas!$D$243</f>
         <v/>
       </c>
       <c r="AA24" s="119">
-        <f>+'[17]Estado$'!$AE$24</f>
+        <f>+'[16]Estado$'!$AE$24</f>
         <v/>
       </c>
       <c r="AB24" s="119">
-        <f>+'[17]Estado$'!$AH$24</f>
+        <f>+'[16]Estado$'!$AH$24</f>
         <v/>
       </c>
       <c r="AC24" s="119">
-        <f>+'[17]Estado$'!$AJ$24</f>
+        <f>+'[16]Estado$'!$AJ$24</f>
         <v/>
       </c>
       <c r="AD24" s="119">
-        <f>+'[17]Estado$'!$AK$24</f>
+        <f>+'[16]Estado$'!$AK$24</f>
         <v/>
       </c>
       <c r="AE24" s="326">
-        <f>+'[17]Estado$'!$AI$24+1</f>
+        <f>+'[16]Estado$'!$AI$24+1</f>
         <v/>
       </c>
       <c r="AF24" s="326">
-        <f>+[11]Estado!$AA$24</f>
+        <f>+[10]Estado!$AA$24</f>
         <v/>
       </c>
       <c r="AH24" s="331">
@@ -9273,13 +8360,11 @@
       <c r="H25" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="129">
-        <f>+[13]Estado!C25</f>
-        <v/>
-      </c>
-      <c r="J25" s="129">
-        <f>+'[15]Estado$'!$AC$25</f>
-        <v/>
+      <c r="I25" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="129" t="n">
+        <v>6059</v>
       </c>
       <c r="K25" s="88" t="n"/>
       <c r="L25" s="129" t="n">
@@ -9333,23 +8418,23 @@
         </is>
       </c>
       <c r="AA25" s="215">
-        <f>+'[5]Estado$'!$AE$25</f>
+        <f>+'[4]Estado$'!$AE$25</f>
         <v/>
       </c>
       <c r="AB25" s="215">
-        <f>+'[5]Estado$'!$AH$25</f>
+        <f>+'[4]Estado$'!$AH$25</f>
         <v/>
       </c>
       <c r="AC25" s="216">
-        <f>+'[5]Estado$'!$AJ$25</f>
+        <f>+'[4]Estado$'!$AJ$25</f>
         <v/>
       </c>
       <c r="AD25" s="217">
-        <f>+'[17]Estado$'!$AK$25</f>
+        <f>+'[16]Estado$'!$AK$25</f>
         <v/>
       </c>
       <c r="AE25" s="215">
-        <f>+'[17]Estado$'!$AI$25</f>
+        <f>+'[16]Estado$'!$AI$25</f>
         <v/>
       </c>
       <c r="AF25" s="218" t="inlineStr">
@@ -9388,13 +8473,11 @@
       <c r="H26" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="129">
-        <f>+[13]Estado!C26</f>
-        <v/>
-      </c>
-      <c r="J26" s="129">
-        <f>+'[15]Estado$'!$AC$26</f>
-        <v/>
+      <c r="I26" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="129" t="n">
+        <v>403110</v>
       </c>
       <c r="K26" s="88" t="n"/>
       <c r="L26" s="129" t="n">
@@ -9470,13 +8553,11 @@
       <c r="H27" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="129">
-        <f>+[13]Estado!C27</f>
-        <v/>
-      </c>
-      <c r="J27" s="129">
-        <f>+'[15]Estado$'!$AC$27</f>
-        <v/>
+      <c r="I27" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="129" t="n">
+        <v>9234185858</v>
       </c>
       <c r="K27" s="88" t="n"/>
       <c r="L27" s="129" t="n">
@@ -9544,13 +8625,11 @@
       <c r="H28" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="129">
-        <f>+[13]Estado!C28</f>
-        <v/>
-      </c>
-      <c r="J28" s="129">
-        <f>+'[15]Estado$'!$AC$28</f>
-        <v/>
+      <c r="I28" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K28" s="88" t="n"/>
       <c r="L28" s="129" t="n">
@@ -9618,13 +8697,11 @@
       <c r="H29" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="129">
-        <f>+[13]Estado!C29</f>
-        <v/>
-      </c>
-      <c r="J29" s="129">
-        <f>+'[15]Estado$'!$AC$29</f>
-        <v/>
+      <c r="I29" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="129" t="n">
+        <v>98063358</v>
       </c>
       <c r="K29" s="88" t="n"/>
       <c r="L29" s="129" t="n">
@@ -9691,13 +8768,11 @@
       <c r="H30" s="129" t="n">
         <v>68798365</v>
       </c>
-      <c r="I30" s="129">
-        <f>+[13]Estado!C30</f>
-        <v/>
-      </c>
-      <c r="J30" s="129">
-        <f>+'[15]Estado$'!$AC$30</f>
-        <v/>
+      <c r="I30" s="129" t="n">
+        <v>3960531</v>
+      </c>
+      <c r="J30" s="129" t="n">
+        <v>1973899479</v>
       </c>
       <c r="K30" s="88" t="n"/>
       <c r="L30" s="129" t="n">
@@ -10028,13 +9103,11 @@
       <c r="H37" s="150" t="n">
         <v>0</v>
       </c>
-      <c r="I37" s="150">
-        <f>+[13]Estado!C37</f>
-        <v/>
-      </c>
-      <c r="J37" s="150">
-        <f>+'[15]Estado$'!$AC$37</f>
-        <v/>
+      <c r="I37" s="150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="150" t="n">
+        <v>558046576</v>
       </c>
       <c r="K37" s="170" t="n"/>
       <c r="L37" s="150" t="n"/>
@@ -10091,13 +9164,11 @@
       <c r="H38" s="129" t="n">
         <v>54248821</v>
       </c>
-      <c r="I38" s="129">
-        <f>+[13]Estado!C38</f>
-        <v/>
-      </c>
-      <c r="J38" s="129">
-        <f>+'[15]Estado$'!$AC$38</f>
-        <v/>
+      <c r="I38" s="129" t="n">
+        <v>35884384</v>
+      </c>
+      <c r="J38" s="129" t="n">
+        <v>5414028694</v>
       </c>
       <c r="K38" s="88" t="n"/>
       <c r="L38" s="142" t="n"/>
@@ -10156,13 +9227,11 @@
       <c r="H39" s="142" t="n">
         <v>0</v>
       </c>
-      <c r="I39" s="142">
-        <f>+[13]Estado!C39</f>
-        <v/>
-      </c>
-      <c r="J39" s="142">
-        <f>+'[15]Estado$'!$AC$39</f>
-        <v/>
+      <c r="I39" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="142" t="n">
+        <v>0</v>
       </c>
       <c r="K39" s="168" t="n"/>
       <c r="L39" s="142" t="n">
@@ -10175,11 +9244,11 @@
         <v>0</v>
       </c>
       <c r="O39" s="142">
-        <f>-[10]Ctas!$D$416</f>
+        <f>-[9]Ctas!$D$416</f>
         <v/>
       </c>
       <c r="P39" s="142">
-        <f>-[11]Estado!$Z$39</f>
+        <f>-[10]Estado!$Z$39</f>
         <v/>
       </c>
       <c r="Q39" s="142" t="n">
@@ -10228,13 +9297,11 @@
       <c r="H40" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I40" s="129">
-        <f>+[13]Estado!C40</f>
-        <v/>
-      </c>
-      <c r="J40" s="129">
-        <f>+'[15]Estado$'!$AC$40</f>
-        <v/>
+      <c r="I40" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="129" t="n">
+        <v>463737719</v>
       </c>
       <c r="K40" s="88" t="n"/>
       <c r="L40" s="129" t="n">
@@ -10296,13 +9363,11 @@
       <c r="H41" s="129" t="n">
         <v>4965044</v>
       </c>
-      <c r="I41" s="129">
-        <f>+[13]Estado!C41</f>
-        <v/>
-      </c>
-      <c r="J41" s="129">
-        <f>+'[15]Estado$'!$AC$41</f>
-        <v/>
+      <c r="I41" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="129" t="n">
+        <v>1112722638</v>
       </c>
       <c r="K41" s="88" t="n"/>
       <c r="L41" s="129" t="n">
@@ -10365,13 +9430,11 @@
       <c r="H42" s="154" t="n">
         <v>254808755</v>
       </c>
-      <c r="I42" s="154">
-        <f>+[13]Estado!C42</f>
-        <v/>
-      </c>
-      <c r="J42" s="154">
-        <f>+'[15]Estado$'!$AC$42</f>
-        <v/>
+      <c r="I42" s="154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="154" t="n">
+        <v>932917018</v>
       </c>
       <c r="K42" s="171" t="n"/>
       <c r="L42" s="154">
@@ -10432,17 +9495,15 @@
       <c r="H43" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I43" s="129">
-        <f>+[13]Estado!C43</f>
-        <v/>
-      </c>
-      <c r="J43" s="129">
-        <f>+'[15]Estado$'!$AC$43</f>
-        <v/>
+      <c r="I43" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="129" t="n">
+        <v>625311782</v>
       </c>
       <c r="K43" s="88" t="n"/>
       <c r="L43" s="142">
-        <f>+'[18]Detalle Cta Cte  Reclasi(Final)'!$BN$57+9647327</f>
+        <f>+'[17]Detalle Cta Cte  Reclasi(Final)'!$BN$57+9647327</f>
         <v/>
       </c>
       <c r="M43" s="142" t="n"/>
@@ -10575,13 +9636,11 @@
       <c r="H45" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I45" s="129">
-        <f>+[13]Estado!C45</f>
-        <v/>
-      </c>
-      <c r="J45" s="129">
-        <f>+'[15]Estado$'!$AC$45</f>
-        <v/>
+      <c r="I45" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K45" s="88" t="n"/>
       <c r="L45" s="129" t="n">
@@ -10747,7 +9806,7 @@
       <c r="U47" s="88" t="n"/>
       <c r="V47" s="126" t="n"/>
       <c r="W47" s="186">
-        <f>+'[5]Estado$'!$AD$47</f>
+        <f>+'[4]Estado$'!$AD$47</f>
         <v/>
       </c>
       <c r="X47" s="186" t="inlineStr">
@@ -10756,7 +9815,7 @@
         </is>
       </c>
       <c r="Y47" s="186">
-        <f>+'[5]Estado$'!$AI$47</f>
+        <f>+'[4]Estado$'!$AI$47</f>
         <v/>
       </c>
       <c r="Z47" s="222" t="inlineStr">
@@ -10809,13 +9868,11 @@
       <c r="H48" s="150" t="n">
         <v>0</v>
       </c>
-      <c r="I48" s="150">
-        <f>+[13]Estado!C48</f>
-        <v/>
-      </c>
-      <c r="J48" s="159">
-        <f>+'[15]Estado$'!$AC$48</f>
-        <v/>
+      <c r="I48" s="150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="159" t="n">
+        <v>4652450566</v>
       </c>
       <c r="K48" s="170" t="n"/>
       <c r="L48" s="150" t="n">
@@ -10825,7 +9882,7 @@
         <v>0</v>
       </c>
       <c r="N48" s="159">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$K$55-'[18]cta cte  (Ajustes) (Final)'!$O$55-'[18]cta cte  (Ajustes) (Final)'!$S$55</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$K$55-'[17]cta cte  (Ajustes) (Final)'!$O$55-'[17]cta cte  (Ajustes) (Final)'!$S$55</f>
         <v/>
       </c>
       <c r="O48" s="150" t="n">
@@ -10841,7 +9898,7 @@
         <v>0</v>
       </c>
       <c r="S48" s="159">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AR$55</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AR$55</f>
         <v/>
       </c>
       <c r="T48" s="150" t="n">
@@ -10853,19 +9910,19 @@
         <v/>
       </c>
       <c r="W48" s="193">
-        <f>+'[18]Cta Cte  (Acumuladas Consol)'!$BJ$54</f>
+        <f>+'[17]Cta Cte  (Acumuladas Consol)'!$BJ$54</f>
         <v/>
       </c>
       <c r="X48" s="193">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$AT$54</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$AT$54</f>
         <v/>
       </c>
       <c r="Y48" s="193">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$AR$54</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$AR$54</f>
         <v/>
       </c>
       <c r="Z48" s="193">
-        <f>+'[18]cta cte  (Final) (Quedan)'!$S$56</f>
+        <f>+'[17]cta cte  (Final) (Quedan)'!$S$56</f>
         <v/>
       </c>
       <c r="AA48" s="193">
@@ -10918,13 +9975,11 @@
       <c r="H49" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I49" s="129">
-        <f>+[13]Estado!C49</f>
-        <v/>
-      </c>
-      <c r="J49" s="129">
-        <f>+'[15]Estado$'!$AC$49</f>
-        <v/>
+      <c r="I49" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="129" t="n">
+        <v>227887275</v>
       </c>
       <c r="K49" s="88" t="n"/>
       <c r="L49" s="132" t="n"/>
@@ -10956,7 +10011,7 @@
       </c>
       <c r="X49" s="194" t="n"/>
       <c r="Y49" s="194">
-        <f>+'[17]Estado$'!$AJ$51</f>
+        <f>+'[16]Estado$'!$AJ$51</f>
         <v/>
       </c>
       <c r="Z49" s="120" t="inlineStr">
@@ -10975,23 +10030,23 @@
         </is>
       </c>
       <c r="AC49" s="194">
-        <f>+'[5]Estado$'!$AE$52</f>
+        <f>+'[4]Estado$'!$AE$52</f>
         <v/>
       </c>
       <c r="AD49" s="194">
-        <f>+'[5]Estado$'!$AF$52</f>
+        <f>+'[4]Estado$'!$AF$52</f>
         <v/>
       </c>
       <c r="AE49" s="194">
-        <f>+'[5]Estado$'!$AG$52</f>
+        <f>+'[4]Estado$'!$AG$52</f>
         <v/>
       </c>
       <c r="AF49" s="119">
-        <f>+'[5]Estado$'!$AH$52</f>
+        <f>+'[4]Estado$'!$AH$52</f>
         <v/>
       </c>
       <c r="AG49" s="119">
-        <f>+'[5]Estado$'!$AI$52</f>
+        <f>+'[4]Estado$'!$AI$52</f>
         <v/>
       </c>
       <c r="AH49" s="192" t="inlineStr">
@@ -11030,44 +10085,42 @@
       <c r="H50" s="142" t="n">
         <v>100000</v>
       </c>
-      <c r="I50" s="142">
-        <f>+[13]Estado!C50</f>
-        <v/>
-      </c>
-      <c r="J50" s="142">
-        <f>+'[15]Estado$'!$AC$50</f>
-        <v/>
+      <c r="I50" s="142" t="n">
+        <v>30646</v>
+      </c>
+      <c r="J50" s="142" t="n">
+        <v>6806005656</v>
       </c>
       <c r="K50" s="88" t="n"/>
       <c r="L50" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$C$43+'[18]cta cte  (Final) (Quedan)'!$BR$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$C$43+'[17]cta cte  (Final) (Quedan)'!$BR$43</f>
         <v/>
       </c>
       <c r="M50" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$E$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$E$43</f>
         <v/>
       </c>
       <c r="N50" s="142" t="n">
         <v>0</v>
       </c>
       <c r="O50" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AB$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AB$43</f>
         <v/>
       </c>
       <c r="P50" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AD$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AD$43</f>
         <v/>
       </c>
       <c r="Q50" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AJ$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AJ$43</f>
         <v/>
       </c>
       <c r="R50" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AL$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AL$43</f>
         <v/>
       </c>
       <c r="S50" s="142">
-        <f>-'[18]cta cte  (Ajustes) (Final)'!$AN$43-'[18]cta cte  (Ajustes) (Final)'!$AX$43-'[18]cta cte  (Ajustes) (Final)'!$BB$43-'[18]cta cte  (Ajustes) (Final)'!$BH$43</f>
+        <f>-'[17]cta cte  (Ajustes) (Final)'!$AN$43-'[17]cta cte  (Ajustes) (Final)'!$AX$43-'[17]cta cte  (Ajustes) (Final)'!$BB$43-'[17]cta cte  (Ajustes) (Final)'!$BH$43</f>
         <v/>
       </c>
       <c r="T50" s="142" t="n">
@@ -11079,48 +10132,48 @@
         <v/>
       </c>
       <c r="W50" s="335">
-        <f>+[7]Ctas!$D$458</f>
+        <f>+[6]Ctas!$D$458</f>
         <v/>
       </c>
       <c r="X50" s="335" t="n"/>
       <c r="Y50" s="225">
-        <f>+'[17]Estado$'!$AJ$50</f>
+        <f>+'[16]Estado$'!$AJ$50</f>
         <v/>
       </c>
       <c r="Z50" s="225">
-        <f>+'[17]Estado$'!$AN$50</f>
+        <f>+'[16]Estado$'!$AN$50</f>
         <v/>
       </c>
       <c r="AA50" s="225">
-        <f>+'[17]Estado$'!$AQ$50</f>
+        <f>+'[16]Estado$'!$AQ$50</f>
         <v/>
       </c>
       <c r="AB50" s="225">
-        <f>+'[17]Estado$'!$AP$50</f>
+        <f>+'[16]Estado$'!$AP$50</f>
         <v/>
       </c>
       <c r="AC50" s="225">
-        <f>+'[17]Estado$'!$AE$50</f>
+        <f>+'[16]Estado$'!$AE$50</f>
         <v/>
       </c>
       <c r="AD50" s="225">
-        <f>+'[17]Estado$'!$AF$50</f>
+        <f>+'[16]Estado$'!$AF$50</f>
         <v/>
       </c>
       <c r="AE50" s="225">
-        <f>+'[17]Estado$'!$AG$50</f>
+        <f>+'[16]Estado$'!$AG$50</f>
         <v/>
       </c>
       <c r="AF50" s="225">
-        <f>+'[17]Estado$'!$AH$50</f>
+        <f>+'[16]Estado$'!$AH$50</f>
         <v/>
       </c>
       <c r="AG50" s="225">
-        <f>+'[17]Estado$'!$AI$50</f>
+        <f>+'[16]Estado$'!$AI$50</f>
         <v/>
       </c>
       <c r="AH50" s="119">
-        <f>+'[17]Estado$'!$AK$50</f>
+        <f>+'[16]Estado$'!$AK$50</f>
         <v/>
       </c>
       <c r="AI50" s="119">
@@ -11157,13 +10210,11 @@
       <c r="H51" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I51" s="129">
-        <f>+[13]Estado!C51</f>
-        <v/>
-      </c>
-      <c r="J51" s="129">
-        <f>+'[15]Estado$'!$AC$51</f>
-        <v/>
+      <c r="I51" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K51" s="88" t="n"/>
       <c r="L51" s="129" t="n">
@@ -11222,13 +10273,11 @@
       <c r="H52" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I52" s="129">
-        <f>+[13]Estado!C52</f>
-        <v/>
-      </c>
-      <c r="J52" s="129">
-        <f>+'[15]Estado$'!$AC$52</f>
-        <v/>
+      <c r="I52" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="129" t="n">
+        <v>1446182627</v>
       </c>
       <c r="K52" s="88" t="n"/>
       <c r="L52" s="129" t="n">
@@ -11287,13 +10336,11 @@
       <c r="H53" s="154" t="n">
         <v>0</v>
       </c>
-      <c r="I53" s="154">
-        <f>+[13]Estado!C53</f>
-        <v/>
-      </c>
-      <c r="J53" s="154">
-        <f>+'[15]Estado$'!$AC$53</f>
-        <v/>
+      <c r="I53" s="154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="154" t="n">
+        <v>0</v>
       </c>
       <c r="K53" s="171" t="n"/>
       <c r="L53" s="154" t="n"/>
@@ -11350,13 +10397,11 @@
       <c r="H54" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I54" s="129">
-        <f>+[13]Estado!C54</f>
-        <v/>
-      </c>
-      <c r="J54" s="129">
-        <f>+'[15]Estado$'!$AC$54</f>
-        <v/>
+      <c r="I54" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="129" t="n">
+        <v>93967634</v>
       </c>
       <c r="K54" s="88" t="n"/>
       <c r="L54" s="132">
@@ -11600,13 +10645,11 @@
       <c r="H58" s="129" t="n">
         <v>1313272</v>
       </c>
-      <c r="I58" s="129">
-        <f>+[13]Estado!C58</f>
-        <v/>
-      </c>
-      <c r="J58" s="129">
-        <f>+'[15]Estado$'!$AC$58</f>
-        <v/>
+      <c r="I58" s="129" t="n">
+        <v>1087339</v>
+      </c>
+      <c r="J58" s="129" t="n">
+        <v>32296318921</v>
       </c>
       <c r="K58" s="88" t="n"/>
       <c r="L58" s="129" t="n">
@@ -11675,13 +10718,11 @@
       <c r="H59" s="129" t="n">
         <v>91438527</v>
       </c>
-      <c r="I59" s="129">
-        <f>+[13]Estado!C59</f>
-        <v/>
-      </c>
-      <c r="J59" s="129">
-        <f>+'[15]Estado$'!$AC$59</f>
-        <v/>
+      <c r="I59" s="129" t="n">
+        <v>160686140</v>
+      </c>
+      <c r="J59" s="129" t="n">
+        <v>7719195458</v>
       </c>
       <c r="K59" s="88" t="n"/>
       <c r="L59" s="129" t="n">
@@ -11750,13 +10791,11 @@
       <c r="H60" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I60" s="129">
-        <f>+[13]Estado!C60</f>
-        <v/>
-      </c>
-      <c r="J60" s="129">
-        <f>+'[15]Estado$'!$AC$60</f>
-        <v/>
+      <c r="I60" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K60" s="88" t="n"/>
       <c r="L60" s="129" t="n">
@@ -11825,13 +10864,11 @@
       <c r="H61" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I61" s="129">
-        <f>+[13]Estado!C61</f>
-        <v/>
-      </c>
-      <c r="J61" s="129">
-        <f>+'[15]Estado$'!$AC$61</f>
-        <v/>
+      <c r="I61" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K61" s="88" t="n"/>
       <c r="L61" s="129" t="n">
@@ -11900,13 +10937,11 @@
       <c r="H62" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I62" s="129">
-        <f>+[13]Estado!C62</f>
-        <v/>
-      </c>
-      <c r="J62" s="129">
-        <f>+'[15]Estado$'!$AC$62</f>
-        <v/>
+      <c r="I62" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" s="129" t="n">
+        <v>0</v>
       </c>
       <c r="K62" s="88" t="n"/>
       <c r="L62" s="129" t="n">
@@ -11975,13 +11010,11 @@
       <c r="H63" s="129" t="n">
         <v>-27011</v>
       </c>
-      <c r="I63" s="129">
-        <f>+[13]Estado!C63</f>
-        <v/>
-      </c>
-      <c r="J63" s="129">
-        <f>+'[15]Estado$'!$AC$63</f>
-        <v/>
+      <c r="I63" s="129" t="n">
+        <v>-22364</v>
+      </c>
+      <c r="J63" s="129" t="n">
+        <v>2488253058</v>
       </c>
       <c r="K63" s="88" t="n"/>
       <c r="L63" s="129" t="n">
@@ -12116,11 +11149,11 @@
         <v/>
       </c>
       <c r="X64" s="197">
-        <f>+'[5]Estado$'!$AE$64</f>
+        <f>+'[4]Estado$'!$AE$64</f>
         <v/>
       </c>
       <c r="Y64" s="197">
-        <f>+'[5]Estado$'!$AG$64</f>
+        <f>+'[4]Estado$'!$AG$64</f>
         <v/>
       </c>
       <c r="Z64" s="197" t="inlineStr">
@@ -12167,19 +11200,17 @@
       <c r="H65" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I65" s="129">
-        <f>+[13]Estado!C65</f>
-        <v/>
-      </c>
-      <c r="J65" s="129">
-        <f>+'[15]Estado$'!$AC$65</f>
-        <v/>
+      <c r="I65" s="129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="129" t="n">
+        <v>4515701</v>
       </c>
       <c r="K65" s="88" t="n"/>
       <c r="L65" s="260" t="n"/>
       <c r="M65" s="261" t="n"/>
       <c r="N65" s="261">
-        <f>-[16]Estado!$AH$65</f>
+        <f>-[15]Estado!$AH$65</f>
         <v/>
       </c>
       <c r="O65" s="261" t="n"/>
@@ -12190,7 +11221,7 @@
       <c r="Q65" s="261" t="n"/>
       <c r="R65" s="261" t="n"/>
       <c r="S65" s="261">
-        <f>-'[17]Estado$'!$AG$65-'[17]Estado$'!$AJ$65-'[17]Estado$'!$AN$65</f>
+        <f>-'[16]Estado$'!$AG$65-'[16]Estado$'!$AJ$65-'[16]Estado$'!$AN$65</f>
         <v/>
       </c>
       <c r="T65" s="261">
@@ -12207,23 +11238,23 @@
         <v/>
       </c>
       <c r="X65" s="268">
-        <f>+'[14]Estado$'!$AD$65</f>
+        <f>+'[13]Estado$'!$AD$65</f>
         <v/>
       </c>
       <c r="Y65" s="268">
-        <f>+'[14]Estado$'!$AF$65</f>
+        <f>+'[13]Estado$'!$AF$65</f>
         <v/>
       </c>
       <c r="Z65" s="337">
-        <f>+[16]Estado!$AG$65</f>
+        <f>+[15]Estado!$AG$65</f>
         <v/>
       </c>
       <c r="AA65" s="337">
-        <f>+[16]Estado!$AB$65</f>
+        <f>+[15]Estado!$AB$65</f>
         <v/>
       </c>
       <c r="AB65" s="119">
-        <f>+'[17]Estado$'!$AI$65</f>
+        <f>+'[16]Estado$'!$AI$65</f>
         <v/>
       </c>
       <c r="AC65" s="334">
@@ -12820,7 +11851,7 @@
       <c r="L75" s="255" t="n"/>
       <c r="M75" s="255" t="n"/>
       <c r="N75" s="255">
-        <f>+'[19]Inversione  (Acumuladas Consol)'!$D$39</f>
+        <f>+'[18]Inversione  (Acumuladas Consol)'!$D$39</f>
         <v/>
       </c>
       <c r="U75" s="275" t="n"/>
@@ -12894,31 +11925,31 @@
       </c>
       <c r="B78" s="122" t="n"/>
       <c r="D78" s="254">
-        <f>+[7]Ctas!$D$238</f>
+        <f>+[6]Ctas!$D$238</f>
         <v/>
       </c>
       <c r="E78" s="254">
-        <f>+[7]Ctas!$D$239</f>
+        <f>+[6]Ctas!$D$239</f>
         <v/>
       </c>
       <c r="F78" s="254">
-        <f>+[7]Ctas!$D$245</f>
+        <f>+[6]Ctas!$D$245</f>
         <v/>
       </c>
       <c r="G78" s="254">
-        <f>+[7]Ctas!$D$242</f>
+        <f>+[6]Ctas!$D$242</f>
         <v/>
       </c>
       <c r="H78" s="254">
-        <f>+[7]Ctas!$D$247</f>
+        <f>+[6]Ctas!$D$247</f>
         <v/>
       </c>
       <c r="I78" s="254">
-        <f>+[7]Ctas!$D$253</f>
+        <f>+[6]Ctas!$D$253</f>
         <v/>
       </c>
       <c r="J78" s="254">
-        <f>+[7]Ctas!$D$246</f>
+        <f>+[6]Ctas!$D$246</f>
         <v/>
       </c>
       <c r="K78" s="88" t="n"/>
@@ -13043,14 +12074,14 @@
       </c>
       <c r="B83" s="122" t="n"/>
       <c r="D83" s="242">
-        <f>+[9]Ctas!$D$209</f>
+        <f>+[8]Ctas!$D$209</f>
         <v/>
       </c>
       <c r="E83" s="242" t="n">
         <v>0</v>
       </c>
       <c r="F83" s="242">
-        <f>+[9]Ctas!$D$216</f>
+        <f>+[8]Ctas!$D$216</f>
         <v/>
       </c>
       <c r="G83" s="242">
@@ -13058,11 +12089,11 @@
         <v/>
       </c>
       <c r="H83" s="242">
-        <f>+[9]Ctas!$D$218</f>
+        <f>+[8]Ctas!$D$218</f>
         <v/>
       </c>
       <c r="I83" s="242">
-        <f>+[9]Ctas!$D$223</f>
+        <f>+[8]Ctas!$D$223</f>
         <v/>
       </c>
       <c r="J83" s="255" t="n"/>
@@ -13654,44 +12685,44 @@
       </c>
       <c r="B5" s="49" t="n"/>
       <c r="C5" s="50">
-        <f>+[7]Resultado!C9</f>
+        <f>+[6]Resultado!C9</f>
         <v/>
       </c>
       <c r="D5" s="50">
-        <f>+[8]Resultado!C5</f>
+        <f>+[7]Resultado!C5</f>
         <v/>
       </c>
       <c r="E5" s="50">
-        <f>+[16]Resultado!Y5</f>
+        <f>+[15]Resultado!Y5</f>
         <v/>
       </c>
       <c r="F5" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="50">
-        <f>+[10]Resultado!$C$5</f>
+        <f>+[9]Resultado!$C$5</f>
         <v/>
       </c>
       <c r="H5" s="50">
-        <f>+[11]Resultado!$Y$5</f>
+        <f>+[10]Resultado!$Y$5</f>
         <v/>
       </c>
       <c r="I5" s="50">
+        <f>+[11]Resultado!C5</f>
+        <v/>
+      </c>
+      <c r="J5" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="50">
         <f>+[12]Resultado!C5</f>
         <v/>
       </c>
-      <c r="J5" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="50">
-        <f>+[13]Resultado!C5</f>
-        <v/>
-      </c>
       <c r="L5" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="50">
-        <f>+'[15]Resultado$'!$AC$5</f>
+        <f>+'[14]Resultado$'!$AC$5</f>
         <v/>
       </c>
       <c r="N5" s="96" t="n"/>
@@ -13704,14 +12735,14 @@
         <v/>
       </c>
       <c r="Q5" s="58">
-        <f>-[16]Resultado!$C$5</f>
+        <f>-[15]Resultado!$C$5</f>
         <v/>
       </c>
       <c r="R5" s="50" t="n">
         <v>0</v>
       </c>
       <c r="T5" s="50">
-        <f>-'[22]Bce Matriz'!$D$511</f>
+        <f>-'[21]Bce Matriz'!$D$511</f>
         <v/>
       </c>
       <c r="U5" s="50">
@@ -13806,44 +12837,44 @@
       </c>
       <c r="B7" s="49" t="n"/>
       <c r="C7" s="50">
-        <f>+[7]Resultado!C11</f>
+        <f>+[6]Resultado!C11</f>
         <v/>
       </c>
       <c r="D7" s="50">
-        <f>+[8]Resultado!C7</f>
+        <f>+[7]Resultado!C7</f>
         <v/>
       </c>
       <c r="E7" s="50">
-        <f>+[16]Resultado!Y7</f>
+        <f>+[15]Resultado!Y7</f>
         <v/>
       </c>
       <c r="F7" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="50">
-        <f>+[10]Resultado!$C$7</f>
+        <f>+[9]Resultado!$C$7</f>
         <v/>
       </c>
       <c r="H7" s="50">
-        <f>+[11]Resultado!$Y$7</f>
+        <f>+[10]Resultado!$Y$7</f>
         <v/>
       </c>
       <c r="I7" s="50">
+        <f>+[11]Resultado!C7</f>
+        <v/>
+      </c>
+      <c r="J7" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="50">
         <f>+[12]Resultado!C7</f>
         <v/>
       </c>
-      <c r="J7" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="50">
-        <f>+[13]Resultado!C7</f>
-        <v/>
-      </c>
       <c r="L7" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="50">
-        <f>+'[15]Resultado$'!$AC$7</f>
+        <f>+'[14]Resultado$'!$AC$7</f>
         <v/>
       </c>
       <c r="N7" s="96" t="n"/>
@@ -14129,44 +13160,44 @@
       </c>
       <c r="B11" s="49" t="n"/>
       <c r="C11" s="50">
-        <f>-[7]Resultado!C15</f>
+        <f>-[6]Resultado!C15</f>
         <v/>
       </c>
       <c r="D11" s="50">
-        <f>-[8]Resultado!C11</f>
+        <f>-[7]Resultado!C11</f>
         <v/>
       </c>
       <c r="E11" s="50">
-        <f>+[16]Resultado!Y11</f>
+        <f>+[15]Resultado!Y11</f>
         <v/>
       </c>
       <c r="F11" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="50">
-        <f>+[10]Resultado!$C$11</f>
+        <f>+[9]Resultado!$C$11</f>
         <v/>
       </c>
       <c r="H11" s="50">
-        <f>+[11]Resultado!$Y$11</f>
+        <f>+[10]Resultado!$Y$11</f>
         <v/>
       </c>
       <c r="I11" s="50">
-        <f>-[12]Resultado!C11</f>
+        <f>-[11]Resultado!C11</f>
         <v/>
       </c>
       <c r="J11" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K11" s="50">
-        <f>+[13]Resultado!C11</f>
+        <f>+[12]Resultado!C11</f>
         <v/>
       </c>
       <c r="L11" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M11" s="50">
-        <f>+'[15]Resultado$'!$AC$11</f>
+        <f>+'[14]Resultado$'!$AC$11</f>
         <v/>
       </c>
       <c r="N11" s="96" t="n"/>
@@ -14249,42 +13280,42 @@
       </c>
       <c r="B12" s="52" t="n"/>
       <c r="C12" s="50">
-        <f>-[7]Resultado!$C$19</f>
+        <f>-[6]Resultado!$C$19</f>
         <v/>
       </c>
       <c r="D12" s="50">
-        <f>+[8]Resultado!C12</f>
+        <f>+[7]Resultado!C12</f>
         <v/>
       </c>
       <c r="E12" s="50">
-        <f>+[16]Resultado!Y12</f>
+        <f>+[15]Resultado!Y12</f>
         <v/>
       </c>
       <c r="F12" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="50">
-        <f>+[10]Resultado!$C$12</f>
+        <f>+[9]Resultado!$C$12</f>
         <v/>
       </c>
       <c r="H12" s="50">
-        <f>+[11]Resultado!$Y$12</f>
+        <f>+[10]Resultado!$Y$12</f>
         <v/>
       </c>
       <c r="I12" s="50">
+        <f>+[11]Resultado!C12</f>
+        <v/>
+      </c>
+      <c r="J12" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="50">
         <f>+[12]Resultado!C12</f>
-        <v/>
-      </c>
-      <c r="J12" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="50">
-        <f>+[13]Resultado!C12</f>
         <v/>
       </c>
       <c r="L12" s="50" t="n"/>
       <c r="M12" s="50">
-        <f>+'[15]Resultado$'!$AC$12</f>
+        <f>+'[14]Resultado$'!$AC$12</f>
         <v/>
       </c>
       <c r="N12" s="96" t="n"/>
@@ -14528,44 +13559,44 @@
       </c>
       <c r="B15" s="49" t="n"/>
       <c r="C15" s="50">
-        <f>+[7]Resultado!$C$23</f>
+        <f>+[6]Resultado!$C$23</f>
         <v/>
       </c>
       <c r="D15" s="50">
-        <f>+[8]Resultado!C15</f>
+        <f>+[7]Resultado!C15</f>
         <v/>
       </c>
       <c r="E15" s="50">
-        <f>+[16]Resultado!Y15</f>
+        <f>+[15]Resultado!Y15</f>
         <v/>
       </c>
       <c r="F15" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="50">
-        <f>+[10]Resultado!$C$15</f>
+        <f>+[9]Resultado!$C$15</f>
         <v/>
       </c>
       <c r="H15" s="50">
-        <f>+[11]Resultado!$Y$15</f>
+        <f>+[10]Resultado!$Y$15</f>
         <v/>
       </c>
       <c r="I15" s="50">
+        <f>+[11]Resultado!C15</f>
+        <v/>
+      </c>
+      <c r="J15" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="50">
         <f>+[12]Resultado!C15</f>
         <v/>
       </c>
-      <c r="J15" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="50">
-        <f>+[13]Resultado!C15</f>
-        <v/>
-      </c>
       <c r="L15" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="50">
-        <f>+'[15]Resultado$'!$AC$15</f>
+        <f>+'[14]Resultado$'!$AC$15</f>
         <v/>
       </c>
       <c r="N15" s="96" t="n"/>
@@ -14637,44 +13668,44 @@
       </c>
       <c r="B17" s="49" t="n"/>
       <c r="C17" s="50">
-        <f>+[7]Resultado!$C$25</f>
+        <f>+[6]Resultado!$C$25</f>
         <v/>
       </c>
       <c r="D17" s="50">
-        <f>+[8]Resultado!C17</f>
+        <f>+[7]Resultado!C17</f>
         <v/>
       </c>
       <c r="E17" s="50">
-        <f>+[16]Resultado!Y17</f>
+        <f>+[15]Resultado!Y17</f>
         <v/>
       </c>
       <c r="F17" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="50">
-        <f>+[10]Resultado!$C$17</f>
+        <f>+[9]Resultado!$C$17</f>
         <v/>
       </c>
       <c r="H17" s="50">
-        <f>+[11]Resultado!$Y$17</f>
+        <f>+[10]Resultado!$Y$17</f>
         <v/>
       </c>
       <c r="I17" s="50">
+        <f>+[11]Resultado!C17</f>
+        <v/>
+      </c>
+      <c r="J17" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="50">
         <f>+[12]Resultado!C17</f>
         <v/>
       </c>
-      <c r="J17" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="50">
-        <f>+[13]Resultado!C17</f>
-        <v/>
-      </c>
       <c r="L17" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M17" s="50">
-        <f>+'[15]Resultado$'!$AC$17</f>
+        <f>+'[14]Resultado$'!$AC$17</f>
         <v/>
       </c>
       <c r="N17" s="96" t="n"/>
@@ -14711,15 +13742,15 @@
         <v/>
       </c>
       <c r="Z17" s="103">
-        <f>+'[5]Resultado$'!$AD$18</f>
+        <f>+'[4]Resultado$'!$AD$18</f>
         <v/>
       </c>
       <c r="AA17" s="103">
-        <f>+'[5]Resultado$'!$AE$18</f>
+        <f>+'[4]Resultado$'!$AE$18</f>
         <v/>
       </c>
       <c r="AB17" s="103">
-        <f>+'[5]Resultado$'!$AF$18</f>
+        <f>+'[4]Resultado$'!$AF$18</f>
         <v/>
       </c>
       <c r="AC17" s="103" t="n"/>
@@ -14783,44 +13814,44 @@
       </c>
       <c r="B19" s="49" t="n"/>
       <c r="C19" s="58">
-        <f>+[7]Resultado!$C$27</f>
+        <f>+[6]Resultado!$C$27</f>
         <v/>
       </c>
       <c r="D19" s="58">
-        <f>+[8]Resultado!C19</f>
+        <f>+[7]Resultado!C19</f>
         <v/>
       </c>
       <c r="E19" s="58">
-        <f>+[16]Resultado!Y19</f>
+        <f>+[15]Resultado!Y19</f>
         <v/>
       </c>
       <c r="F19" s="58" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="58">
-        <f>+[10]Resultado!$C$19</f>
+        <f>+[9]Resultado!$C$19</f>
         <v/>
       </c>
       <c r="H19" s="58">
-        <f>+[11]Resultado!$Y$19</f>
+        <f>+[10]Resultado!$Y$19</f>
         <v/>
       </c>
       <c r="I19" s="58">
+        <f>+[11]Resultado!C19</f>
+        <v/>
+      </c>
+      <c r="J19" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="58">
         <f>+[12]Resultado!C19</f>
         <v/>
       </c>
-      <c r="J19" s="58" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="58">
-        <f>+[13]Resultado!C19</f>
-        <v/>
-      </c>
       <c r="L19" s="58" t="n">
         <v>0</v>
       </c>
       <c r="M19" s="58">
-        <f>+'[15]Resultado$'!$AC$19</f>
+        <f>+'[14]Resultado$'!$AC$19</f>
         <v/>
       </c>
       <c r="N19" s="96" t="n"/>
@@ -14832,7 +13863,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="58">
-        <f>-[16]Resultado!$AI$20</f>
+        <f>-[15]Resultado!$AI$20</f>
         <v/>
       </c>
       <c r="R19" s="58" t="n">
@@ -14860,28 +13891,28 @@
         <v/>
       </c>
       <c r="Z19" s="106">
-        <f>+'[15]Resultado$'!$AD$19</f>
+        <f>+'[14]Resultado$'!$AD$19</f>
         <v/>
       </c>
       <c r="AA19" s="106">
-        <f>+'[15]Resultado$'!$AE$19</f>
+        <f>+'[14]Resultado$'!$AE$19</f>
         <v/>
       </c>
       <c r="AB19" s="106">
-        <f>+'[15]Resultado$'!$AF$19</f>
+        <f>+'[14]Resultado$'!$AF$19</f>
         <v/>
       </c>
       <c r="AC19" s="106" t="n"/>
       <c r="AD19" s="107">
-        <f>+'[20]6220001 Utilidades empresas rel'!$N$17</f>
+        <f>+'[19]6220001 Utilidades empresas rel'!$N$17</f>
         <v/>
       </c>
       <c r="AE19" s="107">
-        <f>+'[20]6220001 Utilidades empresas rel'!$N$16</f>
+        <f>+'[19]6220001 Utilidades empresas rel'!$N$16</f>
         <v/>
       </c>
       <c r="AF19" s="35">
-        <f>-'[21]5220001 Perdidas empresas relac'!$M$15</f>
+        <f>-'[20]5220001 Perdidas empresas relac'!$M$15</f>
         <v/>
       </c>
       <c r="AI19" s="35">
@@ -14929,44 +13960,44 @@
       </c>
       <c r="B21" s="49" t="n"/>
       <c r="C21" s="50">
-        <f>+[7]Resultado!$C$29</f>
+        <f>+[6]Resultado!$C$29</f>
         <v/>
       </c>
       <c r="D21" s="50">
-        <f>+[8]Resultado!C21</f>
+        <f>+[7]Resultado!C21</f>
         <v/>
       </c>
       <c r="E21" s="50">
-        <f>+[16]Resultado!Y21</f>
+        <f>+[15]Resultado!Y21</f>
         <v/>
       </c>
       <c r="F21" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="50">
-        <f>+[10]Resultado!$C$21</f>
+        <f>+[9]Resultado!$C$21</f>
         <v/>
       </c>
       <c r="H21" s="50">
-        <f>+[11]Resultado!$Y$21</f>
+        <f>+[10]Resultado!$Y$21</f>
         <v/>
       </c>
       <c r="I21" s="50">
+        <f>+[11]Resultado!C21</f>
+        <v/>
+      </c>
+      <c r="J21" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="50">
         <f>+[12]Resultado!C21</f>
         <v/>
       </c>
-      <c r="J21" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="50">
-        <f>+[13]Resultado!C21</f>
-        <v/>
-      </c>
       <c r="L21" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M21" s="50">
-        <f>+'[15]Resultado$'!$AC$21</f>
+        <f>+'[14]Resultado$'!$AC$21</f>
         <v/>
       </c>
       <c r="N21" s="96" t="n"/>
@@ -15036,44 +14067,44 @@
       </c>
       <c r="B23" s="49" t="n"/>
       <c r="C23" s="50">
-        <f>+[7]Resultado!$C$31</f>
+        <f>+[6]Resultado!$C$31</f>
         <v/>
       </c>
       <c r="D23" s="50">
-        <f>+[8]Resultado!C23</f>
+        <f>+[7]Resultado!C23</f>
         <v/>
       </c>
       <c r="E23" s="50">
-        <f>+[16]Resultado!Y23</f>
+        <f>+[15]Resultado!Y23</f>
         <v/>
       </c>
       <c r="F23" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="50">
-        <f>+[10]Resultado!$C$23</f>
+        <f>+[9]Resultado!$C$23</f>
         <v/>
       </c>
       <c r="H23" s="50">
-        <f>+[11]Resultado!$Y$23</f>
+        <f>+[10]Resultado!$Y$23</f>
         <v/>
       </c>
       <c r="I23" s="50">
+        <f>+[11]Resultado!C23</f>
+        <v/>
+      </c>
+      <c r="J23" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="50">
         <f>+[12]Resultado!C23</f>
         <v/>
       </c>
-      <c r="J23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="50">
-        <f>+[13]Resultado!C23</f>
-        <v/>
-      </c>
       <c r="L23" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M23" s="50">
-        <f>+'[15]Resultado$'!$AC$23</f>
+        <f>+'[14]Resultado$'!$AC$23</f>
         <v/>
       </c>
       <c r="N23" s="96" t="n"/>
@@ -15137,44 +14168,44 @@
       </c>
       <c r="B25" s="49" t="n"/>
       <c r="C25" s="50">
-        <f>+[7]Resultado!$C$33</f>
+        <f>+[6]Resultado!$C$33</f>
         <v/>
       </c>
       <c r="D25" s="50">
-        <f>+[8]Resultado!C25</f>
+        <f>+[7]Resultado!C25</f>
         <v/>
       </c>
       <c r="E25" s="50">
-        <f>+[16]Resultado!Y25</f>
+        <f>+[15]Resultado!Y25</f>
         <v/>
       </c>
       <c r="F25" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="50">
-        <f>+[10]Resultado!$C$25</f>
+        <f>+[9]Resultado!$C$25</f>
         <v/>
       </c>
       <c r="H25" s="50">
-        <f>+[11]Resultado!$Y$25</f>
+        <f>+[10]Resultado!$Y$25</f>
         <v/>
       </c>
       <c r="I25" s="50">
+        <f>+[11]Resultado!C25</f>
+        <v/>
+      </c>
+      <c r="J25" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="50">
         <f>+[12]Resultado!C25</f>
         <v/>
       </c>
-      <c r="J25" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" s="50">
-        <f>+[13]Resultado!C25</f>
-        <v/>
-      </c>
       <c r="L25" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M25" s="50">
-        <f>+'[15]Resultado$'!$AC$25</f>
+        <f>+'[14]Resultado$'!$AC$25</f>
         <v/>
       </c>
       <c r="N25" s="96" t="n"/>
@@ -15245,44 +14276,44 @@
       </c>
       <c r="B27" s="49" t="n"/>
       <c r="C27" s="50">
-        <f>+[7]Resultado!$C$35</f>
+        <f>+[6]Resultado!$C$35</f>
         <v/>
       </c>
       <c r="D27" s="50">
-        <f>+[8]Resultado!C27</f>
+        <f>+[7]Resultado!C27</f>
         <v/>
       </c>
       <c r="E27" s="50">
-        <f>+[16]Resultado!Y27</f>
+        <f>+[15]Resultado!Y27</f>
         <v/>
       </c>
       <c r="F27" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G27" s="50">
-        <f>+[10]Resultado!$C$27</f>
+        <f>+[9]Resultado!$C$27</f>
         <v/>
       </c>
       <c r="H27" s="50">
-        <f>+[11]Resultado!$Y$27</f>
+        <f>+[10]Resultado!$Y$27</f>
         <v/>
       </c>
       <c r="I27" s="50">
+        <f>+[11]Resultado!C27</f>
+        <v/>
+      </c>
+      <c r="J27" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="50">
         <f>+[12]Resultado!C27</f>
         <v/>
       </c>
-      <c r="J27" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="50">
-        <f>+[13]Resultado!C27</f>
-        <v/>
-      </c>
       <c r="L27" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M27" s="50">
-        <f>+'[15]Resultado$'!$AC$27</f>
+        <f>+'[14]Resultado$'!$AC$27</f>
         <v/>
       </c>
       <c r="N27" s="96" t="n"/>
@@ -15475,44 +14506,44 @@
       </c>
       <c r="B31" s="49" t="n"/>
       <c r="C31" s="50">
-        <f>+[7]Resultado!$C$39</f>
+        <f>+[6]Resultado!$C$39</f>
         <v/>
       </c>
       <c r="D31" s="50">
-        <f>+[8]Resultado!C31</f>
+        <f>+[7]Resultado!C31</f>
         <v/>
       </c>
       <c r="E31" s="50">
-        <f>+[16]Resultado!Y31</f>
+        <f>+[15]Resultado!Y31</f>
         <v/>
       </c>
       <c r="F31" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G31" s="50">
-        <f>+[10]Resultado!$C$31</f>
+        <f>+[9]Resultado!$C$31</f>
         <v/>
       </c>
       <c r="H31" s="50">
-        <f>+[11]Resultado!$Y$31</f>
+        <f>+[10]Resultado!$Y$31</f>
         <v/>
       </c>
       <c r="I31" s="50">
+        <f>+[11]Resultado!C31</f>
+        <v/>
+      </c>
+      <c r="J31" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="50">
         <f>+[12]Resultado!C31</f>
         <v/>
       </c>
-      <c r="J31" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" s="50">
-        <f>+[13]Resultado!C31</f>
-        <v/>
-      </c>
       <c r="L31" s="50" t="n">
         <v>0</v>
       </c>
       <c r="M31" s="50">
-        <f>+'[15]Resultado$'!$AC$31</f>
+        <f>+'[14]Resultado$'!$AC$31</f>
         <v/>
       </c>
       <c r="N31" s="96" t="n"/>
@@ -15713,18 +14744,18 @@
         <v/>
       </c>
       <c r="E35" s="50">
-        <f>+[16]Resultado!Y35</f>
+        <f>+[15]Resultado!Y35</f>
         <v/>
       </c>
       <c r="F35" s="50" t="n">
         <v>0</v>
       </c>
       <c r="G35" s="50">
-        <f>+[10]Resultado!$C$33</f>
+        <f>+[9]Resultado!$C$33</f>
         <v/>
       </c>
       <c r="H35" s="50">
-        <f>+[11]Resultado!$Y$35</f>
+        <f>+[10]Resultado!$Y$35</f>
         <v/>
       </c>
       <c r="I35" s="50">
@@ -15742,7 +14773,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="50">
-        <f>+'[15]Resultado$'!$AC$35</f>
+        <f>+'[14]Resultado$'!$AC$35</f>
         <v/>
       </c>
       <c r="N35" s="99" t="n"/>
@@ -15787,7 +14818,7 @@
         <v/>
       </c>
       <c r="AB35" s="36">
-        <f>+[6]Resultado!$AG$35</f>
+        <f>+[5]Resultado!$AG$35</f>
         <v/>
       </c>
     </row>
@@ -15830,7 +14861,7 @@
       </c>
       <c r="AA36" s="109" t="n"/>
       <c r="AB36" s="110">
-        <f>+[6]Resultado!$AG$36</f>
+        <f>+[5]Resultado!$AG$36</f>
         <v/>
       </c>
       <c r="AC36" s="103" t="inlineStr">
@@ -15839,7 +14870,7 @@
         </is>
       </c>
       <c r="AD36" s="109">
-        <f>+'[5]Resultado$'!$AD$36</f>
+        <f>+'[4]Resultado$'!$AD$36</f>
         <v/>
       </c>
       <c r="AE36" s="109" t="n"/>
@@ -15868,7 +14899,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="50">
-        <f>+[16]Resultado!Y37</f>
+        <f>+[15]Resultado!Y37</f>
         <v/>
       </c>
       <c r="F37" s="50" t="n">
@@ -15879,7 +14910,7 @@
         <v/>
       </c>
       <c r="H37" s="50">
-        <f>+[11]Resultado!$Y$37</f>
+        <f>+[10]Resultado!$Y$37</f>
         <v/>
       </c>
       <c r="I37" s="50" t="n">
@@ -15895,7 +14926,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="50">
-        <f>+'[15]Resultado$'!$AC$37</f>
+        <f>+'[14]Resultado$'!$AC$37</f>
         <v/>
       </c>
       <c r="N37" s="98" t="n"/>
@@ -15904,7 +14935,7 @@
       </c>
       <c r="P37" s="58" t="n"/>
       <c r="Q37" s="58">
-        <f>-[16]Resultado!$AH$37</f>
+        <f>-[15]Resultado!$AH$37</f>
         <v/>
       </c>
       <c r="R37" s="58" t="n"/>
@@ -15916,7 +14947,7 @@
       <c r="U37" s="58" t="n"/>
       <c r="V37" s="58" t="n"/>
       <c r="W37" s="58">
-        <f>-M37+'[15]Resultado$'!$AD$37</f>
+        <f>-M37+'[14]Resultado$'!$AD$37</f>
         <v/>
       </c>
       <c r="X37" s="98" t="n"/>
@@ -15930,15 +14961,15 @@
       </c>
       <c r="AA37" s="112" t="n"/>
       <c r="AB37" s="113">
-        <f>+[16]Resultado!$AG$37</f>
+        <f>+[15]Resultado!$AG$37</f>
         <v/>
       </c>
       <c r="AC37" s="113">
-        <f>+[6]Resultado!$AD$37</f>
+        <f>+[5]Resultado!$AD$37</f>
         <v/>
       </c>
       <c r="AD37" s="113">
-        <f>+'[14]Resultado$'!$AD$37</f>
+        <f>+'[13]Resultado$'!$AD$37</f>
         <v/>
       </c>
       <c r="AE37" s="112" t="n"/>
@@ -16488,40 +15519,40 @@
         </is>
       </c>
       <c r="D50" s="82">
-        <f>+'[20]6220001 Utilidades empresas rel'!$N$13</f>
+        <f>+'[19]6220001 Utilidades empresas rel'!$N$13</f>
         <v/>
       </c>
       <c r="E50" s="82">
-        <f>-'[21]5220001 Perdidas empresas relac'!$M$13</f>
+        <f>-'[20]5220001 Perdidas empresas relac'!$M$13</f>
         <v/>
       </c>
       <c r="F50" s="82" t="n">
         <v>0</v>
       </c>
       <c r="G50" s="82">
-        <f>+'[20]6220001 Utilidades empresas rel'!$N$14</f>
+        <f>+'[19]6220001 Utilidades empresas rel'!$N$14</f>
         <v/>
       </c>
       <c r="H50" s="82">
-        <f>+'[20]6220001 Utilidades empresas rel'!$N$15</f>
+        <f>+'[19]6220001 Utilidades empresas rel'!$N$15</f>
         <v/>
       </c>
       <c r="I50" s="82">
-        <f>-'[21]5220001 Perdidas empresas relac'!$M$12</f>
+        <f>-'[20]5220001 Perdidas empresas relac'!$M$12</f>
         <v/>
       </c>
       <c r="J50" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K50" s="82">
-        <f>+'[20]6220001 Utilidades empresas rel'!$N$12</f>
+        <f>+'[19]6220001 Utilidades empresas rel'!$N$12</f>
         <v/>
       </c>
       <c r="L50" s="82" t="n">
         <v>0</v>
       </c>
       <c r="M50" s="82">
-        <f>-'[21]5220001 Perdidas empresas relac'!$M$14</f>
+        <f>-'[20]5220001 Perdidas empresas relac'!$M$14</f>
         <v/>
       </c>
       <c r="O50" s="47">
@@ -16609,22 +15640,22 @@
     </row>
     <row r="54">
       <c r="D54" s="47">
-        <f>+[16]Resultado!$AG$20</f>
+        <f>+[15]Resultado!$AG$20</f>
         <v/>
       </c>
       <c r="G54" s="47">
-        <f>+[16]Resultado!$Z$20</f>
+        <f>+[15]Resultado!$Z$20</f>
         <v/>
       </c>
       <c r="H54" s="34" t="n">
         <v>0</v>
       </c>
       <c r="I54" s="47">
-        <f>+[16]Resultado!$AD$20</f>
+        <f>+[15]Resultado!$AD$20</f>
         <v/>
       </c>
       <c r="K54" s="47">
-        <f>+[16]Resultado!$AE$20</f>
+        <f>+[15]Resultado!$AE$20</f>
         <v/>
       </c>
       <c r="O54" s="47">
@@ -24179,7 +23210,7 @@
         </is>
       </c>
       <c r="C3" s="2">
-        <f>+[4]Ctas!$D$193</f>
+        <f>+[3]Ctas!$D$193</f>
         <v/>
       </c>
       <c r="D3" s="23" t="n"/>
@@ -24208,7 +23239,7 @@
         </is>
       </c>
       <c r="C4" s="2">
-        <f>+[4]Ctas!$D$196</f>
+        <f>+[3]Ctas!$D$196</f>
         <v/>
       </c>
       <c r="D4" s="24" t="n">
@@ -24241,7 +23272,7 @@
         </is>
       </c>
       <c r="C5" s="2">
-        <f>+[4]Ctas!$D$197</f>
+        <f>+[3]Ctas!$D$197</f>
         <v/>
       </c>
       <c r="D5" s="2" t="n">
@@ -24274,7 +23305,7 @@
         </is>
       </c>
       <c r="C6" s="2">
-        <f>+[4]Ctas!$D$198</f>
+        <f>+[3]Ctas!$D$198</f>
         <v/>
       </c>
       <c r="D6" s="2" t="n">
@@ -24369,7 +23400,7 @@
         </is>
       </c>
       <c r="C9" s="2">
-        <f>+[4]Ctas!$D$206</f>
+        <f>+[3]Ctas!$D$206</f>
         <v/>
       </c>
       <c r="D9" s="2" t="n">
@@ -24401,7 +23432,7 @@
         </is>
       </c>
       <c r="C10" s="2">
-        <f>+[4]Ctas!$D$207</f>
+        <f>+[3]Ctas!$D$207</f>
         <v/>
       </c>
       <c r="D10" s="2" t="n"/>
@@ -24460,7 +23491,7 @@
         </is>
       </c>
       <c r="C12" s="2">
-        <f>+[4]Ctas!$D$210</f>
+        <f>+[3]Ctas!$D$210</f>
         <v/>
       </c>
       <c r="D12" s="2" t="n"/>
@@ -24488,7 +23519,7 @@
         </is>
       </c>
       <c r="C13" s="2">
-        <f>+[4]Ctas!$D$213</f>
+        <f>+[3]Ctas!$D$213</f>
         <v/>
       </c>
       <c r="D13" s="2" t="n">
@@ -24555,7 +23586,7 @@
         </is>
       </c>
       <c r="C15" s="2">
-        <f>+[4]Ctas!$D$217</f>
+        <f>+[3]Ctas!$D$217</f>
         <v/>
       </c>
       <c r="D15" s="2" t="n"/>
@@ -24583,7 +23614,7 @@
         </is>
       </c>
       <c r="C16" s="2">
-        <f>+[4]Ctas!$D$219</f>
+        <f>+[3]Ctas!$D$219</f>
         <v/>
       </c>
       <c r="D16" s="2" t="n">
@@ -24622,7 +23653,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <f>+'[17]Estado$'!$D$215</f>
+        <f>+'[16]Estado$'!$D$215</f>
         <v/>
       </c>
       <c r="E17" s="2">
@@ -24656,7 +23687,7 @@
         </is>
       </c>
       <c r="C18" s="2">
-        <f>+[4]Ctas!$D$226</f>
+        <f>+[3]Ctas!$D$226</f>
         <v/>
       </c>
       <c r="D18" s="2" t="n">
@@ -24688,7 +23719,7 @@
         </is>
       </c>
       <c r="C19" s="2">
-        <f>+[4]Ctas!$D$230</f>
+        <f>+[3]Ctas!$D$230</f>
         <v/>
       </c>
       <c r="D19" s="2" t="n"/>
@@ -24741,7 +23772,7 @@
         </is>
       </c>
       <c r="C21" s="2">
-        <f>+[4]Ctas!$D$223</f>
+        <f>+[3]Ctas!$D$223</f>
         <v/>
       </c>
       <c r="D21" s="2" t="n"/>
@@ -24769,7 +23800,7 @@
         </is>
       </c>
       <c r="C22" s="2">
-        <f>+[4]Ctas!$D$228</f>
+        <f>+[3]Ctas!$D$228</f>
         <v/>
       </c>
       <c r="D22" s="2" t="n"/>
@@ -24797,7 +23828,7 @@
         </is>
       </c>
       <c r="C23" s="2">
-        <f>+[4]Ctas!$D$232</f>
+        <f>+[3]Ctas!$D$232</f>
         <v/>
       </c>
       <c r="D23" s="2" t="n"/>
@@ -24825,7 +23856,7 @@
         </is>
       </c>
       <c r="C24" s="2">
-        <f>+[4]Ctas!$D$231</f>
+        <f>+[3]Ctas!$D$231</f>
         <v/>
       </c>
       <c r="D24" s="2" t="n"/>
@@ -25071,7 +24102,7 @@
     </row>
     <row r="34">
       <c r="C34" s="2">
-        <f>+[4]Ctas!$D$232</f>
+        <f>+[3]Ctas!$D$232</f>
         <v/>
       </c>
       <c r="D34" s="2" t="n"/>
@@ -25251,7 +24282,7 @@
         </is>
       </c>
       <c r="C40" s="2">
-        <f>+[4]Ctas!$D$448</f>
+        <f>+[3]Ctas!$D$448</f>
         <v/>
       </c>
       <c r="M40" s="2">
@@ -25271,7 +24302,7 @@
         </is>
       </c>
       <c r="C41" s="2">
-        <f>+[4]Ctas!$D$449</f>
+        <f>+[3]Ctas!$D$449</f>
         <v/>
       </c>
       <c r="M41" s="2" t="n"/>
@@ -25288,7 +24319,7 @@
         </is>
       </c>
       <c r="C42" s="2">
-        <f>+[4]Ctas!$D$450</f>
+        <f>+[3]Ctas!$D$450</f>
         <v/>
       </c>
       <c r="M42" s="2" t="n"/>
@@ -25305,7 +24336,7 @@
         </is>
       </c>
       <c r="C43" s="2">
-        <f>+[4]Ctas!$D$451</f>
+        <f>+[3]Ctas!$D$451</f>
         <v/>
       </c>
       <c r="M43" s="2" t="n"/>
@@ -25322,7 +24353,7 @@
         </is>
       </c>
       <c r="C44" s="2">
-        <f>+[4]Ctas!$D$452</f>
+        <f>+[3]Ctas!$D$452</f>
         <v/>
       </c>
       <c r="E44" s="2">
@@ -25350,7 +24381,7 @@
         </is>
       </c>
       <c r="C45" s="2">
-        <f>+[4]Ctas!$D$454</f>
+        <f>+[3]Ctas!$D$454</f>
         <v/>
       </c>
       <c r="E45" s="2" t="n"/>
@@ -25374,7 +24405,7 @@
         </is>
       </c>
       <c r="C46" s="2">
-        <f>+[4]Ctas!$D$462</f>
+        <f>+[3]Ctas!$D$462</f>
         <v/>
       </c>
       <c r="H46" s="2" t="n"/>
@@ -25395,7 +24426,7 @@
         </is>
       </c>
       <c r="C47" s="2">
-        <f>+[4]Ctas!$D$463</f>
+        <f>+[3]Ctas!$D$463</f>
         <v/>
       </c>
       <c r="M47" s="2">
@@ -25415,7 +24446,7 @@
         </is>
       </c>
       <c r="C48" s="2">
-        <f>+[4]Ctas!$D$465</f>
+        <f>+[3]Ctas!$D$465</f>
         <v/>
       </c>
       <c r="M48" s="2" t="n"/>
@@ -25432,7 +24463,7 @@
         </is>
       </c>
       <c r="C49" s="2">
-        <f>+[4]Ctas!$D$466</f>
+        <f>+[3]Ctas!$D$466</f>
         <v/>
       </c>
       <c r="M49" s="2" t="n"/>
@@ -25449,7 +24480,7 @@
         </is>
       </c>
       <c r="C50" s="2">
-        <f>+[4]Ctas!$D$467</f>
+        <f>+[3]Ctas!$D$467</f>
         <v/>
       </c>
       <c r="M50" s="2" t="n"/>
@@ -25466,7 +24497,7 @@
         </is>
       </c>
       <c r="C51" s="2">
-        <f>+[4]Ctas!$D$469</f>
+        <f>+[3]Ctas!$D$469</f>
         <v/>
       </c>
       <c r="M51" s="2" t="n"/>
@@ -25483,7 +24514,7 @@
         </is>
       </c>
       <c r="C52" s="2">
-        <f>+[4]Ctas!$D$471</f>
+        <f>+[3]Ctas!$D$471</f>
         <v/>
       </c>
       <c r="M52" s="2" t="n"/>
@@ -25500,7 +24531,7 @@
         </is>
       </c>
       <c r="C53" s="2">
-        <f>+[4]Ctas!$D$473</f>
+        <f>+[3]Ctas!$D$473</f>
         <v/>
       </c>
       <c r="M53" s="2">
@@ -27970,7 +27001,7 @@
         </is>
       </c>
       <c r="C3" s="2">
-        <f>+[4]Ctas!$D$240</f>
+        <f>+[3]Ctas!$D$240</f>
         <v/>
       </c>
       <c r="D3" s="2" t="n">
@@ -28054,7 +27085,7 @@
         </is>
       </c>
       <c r="C5" s="2">
-        <f>+[4]Ctas!$D$237</f>
+        <f>+[3]Ctas!$D$237</f>
         <v/>
       </c>
       <c r="D5" s="2" t="n">
@@ -28304,7 +27335,7 @@
         </is>
       </c>
       <c r="C11" s="2">
-        <f>+[4]Ctas!$D$246</f>
+        <f>+[3]Ctas!$D$246</f>
         <v/>
       </c>
       <c r="D11" s="2" t="n"/>
@@ -28325,7 +27356,7 @@
         </is>
       </c>
       <c r="C12" s="2">
-        <f>+[4]Ctas!$D$249</f>
+        <f>+[3]Ctas!$D$249</f>
         <v/>
       </c>
       <c r="D12" s="2" t="n">

</xml_diff>

<commit_message>
cambios en botones y estructura
</commit_message>
<xml_diff>
--- a/recursos/planilla_standard.xlsx
+++ b/recursos/planilla_standard.xlsx
@@ -6715,7 +6715,7 @@
       </c>
       <c r="B6" s="122" t="n"/>
       <c r="C6" s="129" t="n">
-        <v>3991436469</v>
+        <v>0</v>
       </c>
       <c r="D6" s="129" t="n">
         <v>3117802</v>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="B7" s="122" t="n"/>
       <c r="C7" s="129" t="n">
-        <v>0</v>
+        <v>3255872574.56</v>
       </c>
       <c r="D7" s="129" t="n">
         <v>0</v>
@@ -6841,7 +6841,7 @@
       </c>
       <c r="B8" s="122" t="n"/>
       <c r="C8" s="129" t="n">
-        <v>28670407</v>
+        <v>0</v>
       </c>
       <c r="D8" s="129" t="n">
         <v>0</v>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="B9" s="122" t="n"/>
       <c r="C9" s="129" t="n">
-        <v>544775395</v>
+        <v>2982274761.46</v>
       </c>
       <c r="D9" s="129" t="n">
         <v>2340104</v>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="B10" s="131" t="n"/>
       <c r="C10" s="132" t="n">
-        <v>0</v>
+        <v>60073559317.1884</v>
       </c>
       <c r="D10" s="132" t="n">
         <v>0</v>
@@ -7037,7 +7037,7 @@
       </c>
       <c r="B11" s="122" t="n"/>
       <c r="C11" s="129" t="n">
-        <v>53135152</v>
+        <v>0</v>
       </c>
       <c r="D11" s="129" t="n">
         <v>0</v>
@@ -7163,7 +7163,7 @@
       </c>
       <c r="B13" s="122" t="n"/>
       <c r="C13" s="129" t="n">
-        <v>668517589</v>
+        <v>0</v>
       </c>
       <c r="D13" s="129" t="n">
         <v>0</v>
@@ -7305,7 +7305,7 @@
       </c>
       <c r="B15" s="122" t="n"/>
       <c r="C15" s="129" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="D15" s="129" t="n">
         <v>0</v>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="B16" s="122" t="n"/>
       <c r="C16" s="129" t="n">
-        <v>0</v>
+        <v>10397155079.081</v>
       </c>
       <c r="D16" s="129" t="n">
         <v>0</v>
@@ -7676,7 +7676,7 @@
       </c>
       <c r="B20" s="122" t="n"/>
       <c r="C20" s="139" t="n">
-        <v>0</v>
+        <v>5414956957.90246</v>
       </c>
       <c r="D20" s="139" t="n">
         <v>0</v>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="B21" s="122" t="n"/>
       <c r="C21" s="129" t="n">
-        <v>7244332690</v>
+        <v>1080749265</v>
       </c>
       <c r="D21" s="129" t="n">
         <v>0</v>
@@ -7888,7 +7888,7 @@
       </c>
       <c r="B22" s="122" t="n"/>
       <c r="C22" s="129" t="n">
-        <v>0</v>
+        <v>2322931563</v>
       </c>
       <c r="D22" s="129" t="n">
         <v>0</v>
@@ -8054,7 +8054,7 @@
       </c>
       <c r="B23" s="122" t="n"/>
       <c r="C23" s="142" t="n">
-        <v>3706892400</v>
+        <v>17700987132.42</v>
       </c>
       <c r="D23" s="142" t="n">
         <v>212649967</v>
@@ -8223,7 +8223,7 @@
       </c>
       <c r="B24" s="122" t="n"/>
       <c r="C24" s="144" t="n">
-        <v>66927963658</v>
+        <v>0</v>
       </c>
       <c r="D24" s="144" t="n">
         <v>0</v>
@@ -8343,7 +8343,7 @@
       </c>
       <c r="B25" s="122" t="n"/>
       <c r="C25" s="129" t="n">
-        <v>0</v>
+        <v>2106581917.46</v>
       </c>
       <c r="D25" s="129" t="n">
         <v>0</v>
@@ -8456,7 +8456,7 @@
       </c>
       <c r="B26" s="122" t="n"/>
       <c r="C26" s="129" t="n">
-        <v>0</v>
+        <v>2366980990</v>
       </c>
       <c r="D26" s="129" t="n">
         <v>0</v>
@@ -8536,7 +8536,7 @@
       </c>
       <c r="B27" s="122" t="n"/>
       <c r="C27" s="129" t="n">
-        <v>7219481303</v>
+        <v>52410709330.2726</v>
       </c>
       <c r="D27" s="129" t="n">
         <v>0</v>
@@ -8608,7 +8608,7 @@
       </c>
       <c r="B28" s="122" t="n"/>
       <c r="C28" s="129" t="n">
-        <v>0</v>
+        <v>112484268647.461</v>
       </c>
       <c r="D28" s="129" t="n">
         <v>0</v>
@@ -8680,7 +8680,7 @@
       </c>
       <c r="B29" s="122" t="n"/>
       <c r="C29" s="129" t="n">
-        <v>1221545875</v>
+        <v/>
       </c>
       <c r="D29" s="129" t="n">
         <v>0</v>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="B30" s="122" t="n"/>
       <c r="C30" s="129" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="D30" s="129" t="n">
         <v>7393024</v>
@@ -9086,7 +9086,7 @@
       </c>
       <c r="B37" s="122" t="n"/>
       <c r="C37" s="150" t="n">
-        <v>409483261</v>
+        <v>1528704399</v>
       </c>
       <c r="D37" s="150" t="n">
         <v>0</v>
@@ -9147,7 +9147,7 @@
       </c>
       <c r="B38" s="122" t="n"/>
       <c r="C38" s="129" t="n">
-        <v>556915101</v>
+        <v>1329297676</v>
       </c>
       <c r="D38" s="129" t="n">
         <v>1099353</v>
@@ -9210,7 +9210,7 @@
       </c>
       <c r="B39" s="152" t="n"/>
       <c r="C39" s="142" t="n">
-        <v>0</v>
+        <v>1914548429.67</v>
       </c>
       <c r="D39" s="142" t="n">
         <v>0</v>
@@ -9280,7 +9280,7 @@
       </c>
       <c r="B40" s="122" t="n"/>
       <c r="C40" s="129" t="n">
-        <v>0</v>
+        <v>21211340836.73</v>
       </c>
       <c r="D40" s="129" t="n">
         <v>0</v>
@@ -9346,7 +9346,7 @@
       </c>
       <c r="B41" s="122" t="n"/>
       <c r="C41" s="129" t="n">
-        <v>74649635</v>
+        <v>0</v>
       </c>
       <c r="D41" s="129" t="n">
         <v>0</v>
@@ -9413,7 +9413,7 @@
       </c>
       <c r="B42" s="122" t="n"/>
       <c r="C42" s="154" t="n">
-        <v>0</v>
+        <v>19739852323.73</v>
       </c>
       <c r="D42" s="154" t="n">
         <v>0</v>
@@ -9478,7 +9478,7 @@
       </c>
       <c r="B43" s="122" t="n"/>
       <c r="C43" s="129" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="D43" s="129" t="n">
         <v>0</v>
@@ -9619,7 +9619,7 @@
       </c>
       <c r="B45" s="122" t="n"/>
       <c r="C45" s="129" t="n">
-        <v>0</v>
+        <v>908295196</v>
       </c>
       <c r="D45" s="129" t="n">
         <v>0</v>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="B48" s="158" t="n"/>
       <c r="C48" s="150" t="n">
-        <v>783863096</v>
+        <v>2571353491</v>
       </c>
       <c r="D48" s="150" t="n">
         <v>0</v>
@@ -10068,7 +10068,7 @@
       </c>
       <c r="B50" s="122" t="n"/>
       <c r="C50" s="142" t="n">
-        <v>6473472320</v>
+        <v>1183222441</v>
       </c>
       <c r="D50" s="142" t="n">
         <v>91754</v>
@@ -10193,7 +10193,7 @@
       </c>
       <c r="B51" s="122" t="n"/>
       <c r="C51" s="129" t="n">
-        <v>0</v>
+        <v>9096048867.27738</v>
       </c>
       <c r="D51" s="129" t="n">
         <v>0</v>
@@ -10256,7 +10256,7 @@
       </c>
       <c r="B52" s="122" t="n"/>
       <c r="C52" s="129" t="n">
-        <v>949215459</v>
+        <v>30307389704.0074</v>
       </c>
       <c r="D52" s="129" t="n">
         <v>0</v>
@@ -10319,7 +10319,7 @@
       </c>
       <c r="B53" s="160" t="n"/>
       <c r="C53" s="154" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="D53" s="154" t="n">
         <v>0</v>
@@ -10380,7 +10380,7 @@
       </c>
       <c r="B54" s="122" t="n"/>
       <c r="C54" s="129" t="n">
-        <v>180959611</v>
+        <v>28743629969</v>
       </c>
       <c r="D54" s="129" t="n">
         <v>0</v>
@@ -10628,7 +10628,7 @@
       </c>
       <c r="B58" s="122" t="n"/>
       <c r="C58" s="129" t="n">
-        <v>28743629969</v>
+        <v>0</v>
       </c>
       <c r="D58" s="129" t="n">
         <v>89385225</v>
@@ -10701,7 +10701,7 @@
       </c>
       <c r="B59" s="122" t="n"/>
       <c r="C59" s="129" t="n">
-        <v>51023010062</v>
+        <v>-8280773107.3422</v>
       </c>
       <c r="D59" s="129" t="n">
         <v>98349992</v>
@@ -10774,7 +10774,7 @@
       </c>
       <c r="B60" s="122" t="n"/>
       <c r="C60" s="129" t="n">
-        <v>0</v>
+        <v>82583297861.65781</v>
       </c>
       <c r="D60" s="129" t="n">
         <v>0</v>
@@ -10847,7 +10847,7 @@
       </c>
       <c r="B61" s="122" t="n"/>
       <c r="C61" s="129" t="n">
-        <v>0</v>
+        <v>-406418917.791066</v>
       </c>
       <c r="D61" s="129" t="n">
         <v>0</v>
@@ -10920,7 +10920,7 @@
       </c>
       <c r="B62" s="122" t="n"/>
       <c r="C62" s="129" t="n">
-        <v>0</v>
+        <v>82903158354.8102</v>
       </c>
       <c r="D62" s="129" t="n">
         <v>0</v>
@@ -10993,7 +10993,7 @@
       </c>
       <c r="B63" s="122" t="n"/>
       <c r="C63" s="129" t="n">
-        <v>2411552424</v>
+        <v>112484268647.874</v>
       </c>
       <c r="D63" s="129" t="n">
         <v>36574573</v>

</xml_diff>